<commit_message>
Update Results - First and Second Plate 3 reps.xlsx
</commit_message>
<xml_diff>
--- a/data/First_round_results/Results - First and Second Plate 3 reps.xlsx
+++ b/data/First_round_results/Results - First and Second Plate 3 reps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOL428\Documents\GitHub\SynbioML\data\First_round_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF9E102-D3AC-4AD9-B58E-6FF1751CB235}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5C735A-D6FE-4EC9-BBA6-762D2CB0BEE3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-2150" windowWidth="25820" windowHeight="14020" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GFPOD" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="473">
   <si>
     <t>RBS</t>
   </si>
@@ -1451,6 +1451,15 @@
   </si>
   <si>
     <t>1,2,3</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>bps_noncore</t>
+  </si>
+  <si>
+    <t>bps_core</t>
   </si>
 </sst>
 </file>
@@ -1586,7 +1595,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -1598,13 +1607,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13179,8 +13181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B66" workbookViewId="0">
-      <selection activeCell="Q175" sqref="Q175"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13278,23 +13280,23 @@
         <v>69.563244149086913</v>
       </c>
       <c r="I2">
-        <f>AVERAGE(D2,F2,G2)</f>
+        <f t="shared" ref="I2:I33" si="0">AVERAGE(D2,F2,G2)</f>
         <v>56.058693581811532</v>
       </c>
       <c r="J2">
-        <f>_xlfn.STDEV.P(D2,F2,G2)</f>
+        <f t="shared" ref="J2:J33" si="1">_xlfn.STDEV.P(D2,F2,G2)</f>
         <v>3.9982461493813499</v>
       </c>
       <c r="K2">
-        <f>_xlfn.STDEV.P(C2:G2)</f>
+        <f t="shared" ref="K2:K33" si="2">_xlfn.STDEV.P(C2:G2)</f>
         <v>17.743662160149835</v>
       </c>
       <c r="L2" s="4">
-        <f>K2/H2</f>
+        <f t="shared" ref="L2:L33" si="3">K2/H2</f>
         <v>0.25507237877120686</v>
       </c>
       <c r="M2" t="s">
-        <v>363</v>
+        <v>470</v>
       </c>
       <c r="N2" t="s">
         <v>466</v>
@@ -13335,27 +13337,27 @@
         <v>45.432031622390497</v>
       </c>
       <c r="H3">
-        <f>AVERAGE(C3:F3)</f>
+        <f t="shared" ref="H3:H8" si="4">AVERAGE(C3:F3)</f>
         <v>55.397221273248171</v>
       </c>
       <c r="I3">
-        <f>AVERAGE(D3,F3,G3)</f>
+        <f t="shared" si="0"/>
         <v>42.515945571794397</v>
       </c>
       <c r="J3">
-        <f>_xlfn.STDEV.P(D3,F3,G3)</f>
+        <f t="shared" si="1"/>
         <v>2.2132627213858149</v>
       </c>
       <c r="K3">
-        <f>_xlfn.STDEV.P(C3:G3)</f>
+        <f t="shared" si="2"/>
         <v>15.256165999900897</v>
       </c>
       <c r="L3" s="4">
-        <f>K3/H3</f>
+        <f t="shared" si="3"/>
         <v>0.2753958709345633</v>
       </c>
       <c r="M3" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N3" t="s">
         <v>466</v>
@@ -13396,27 +13398,27 @@
         <v>24.133637075311899</v>
       </c>
       <c r="H4">
-        <f>AVERAGE(C4:F4)</f>
+        <f t="shared" si="4"/>
         <v>37.715864765628751</v>
       </c>
       <c r="I4">
-        <f>AVERAGE(D4,F4,G4)</f>
+        <f t="shared" si="0"/>
         <v>25.817688712608966</v>
       </c>
       <c r="J4">
-        <f>_xlfn.STDEV.P(D4,F4,G4)</f>
+        <f t="shared" si="1"/>
         <v>2.136029223214535</v>
       </c>
       <c r="K4">
-        <f>_xlfn.STDEV.P(C4:G4)</f>
+        <f t="shared" si="2"/>
         <v>13.004783179702333</v>
       </c>
       <c r="L4" s="4">
-        <f>K4/H4</f>
+        <f t="shared" si="3"/>
         <v>0.34480935968234411</v>
       </c>
       <c r="M4" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N4" t="s">
         <v>466</v>
@@ -13457,27 +13459,27 @@
         <v>38.049576803906</v>
       </c>
       <c r="H5">
-        <f>AVERAGE(C5:F5)</f>
+        <f t="shared" si="4"/>
         <v>54.265356811104148</v>
       </c>
       <c r="I5">
-        <f>AVERAGE(D5,F5,G5)</f>
+        <f t="shared" si="0"/>
         <v>39.928298016107533</v>
       </c>
       <c r="J5">
-        <f>_xlfn.STDEV.P(D5,F5,G5)</f>
+        <f t="shared" si="1"/>
         <v>2.2510645272917604</v>
       </c>
       <c r="K5">
-        <f>_xlfn.STDEV.P(C5:G5)</f>
+        <f t="shared" si="2"/>
         <v>14.385070191384047</v>
       </c>
       <c r="L5" s="4">
-        <f>K5/H5</f>
+        <f t="shared" si="3"/>
         <v>0.26508754455366401</v>
       </c>
       <c r="M5" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N5" t="s">
         <v>466</v>
@@ -13518,27 +13520,27 @@
         <v>38.394865293671302</v>
       </c>
       <c r="H6">
-        <f>AVERAGE(C6:F6)</f>
+        <f t="shared" si="4"/>
         <v>54.724326261503748</v>
       </c>
       <c r="I6">
-        <f>AVERAGE(D6,F6,G6)</f>
+        <f t="shared" si="0"/>
         <v>42.887003446562098</v>
       </c>
       <c r="J6">
-        <f>_xlfn.STDEV.P(D6,F6,G6)</f>
+        <f t="shared" si="1"/>
         <v>3.2396603861831648</v>
       </c>
       <c r="K6">
-        <f>_xlfn.STDEV.P(C6:G6)</f>
+        <f t="shared" si="2"/>
         <v>11.487255342721955</v>
       </c>
       <c r="L6" s="4">
-        <f>K6/H6</f>
+        <f t="shared" si="3"/>
         <v>0.20991131599920224</v>
       </c>
       <c r="M6" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N6" t="s">
         <v>466</v>
@@ -13579,27 +13581,27 @@
         <v>21.1722417929108</v>
       </c>
       <c r="H7">
-        <f>AVERAGE(C7:F7)</f>
+        <f t="shared" si="4"/>
         <v>30.426541897719773</v>
       </c>
       <c r="I7">
-        <f>AVERAGE(D7,F7,G7)</f>
+        <f t="shared" si="0"/>
         <v>21.450546461263301</v>
       </c>
       <c r="J7">
-        <f>_xlfn.STDEV.P(D7,F7,G7)</f>
+        <f t="shared" si="1"/>
         <v>0.37019041536311503</v>
       </c>
       <c r="K7">
-        <f>_xlfn.STDEV.P(C7:G7)</f>
+        <f t="shared" si="2"/>
         <v>10.233622543356331</v>
       </c>
       <c r="L7" s="4">
-        <f>K7/H7</f>
+        <f t="shared" si="3"/>
         <v>0.33633866700189347</v>
       </c>
       <c r="M7" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N7" t="s">
         <v>466</v>
@@ -13640,27 +13642,27 @@
         <v>31.848505915259601</v>
       </c>
       <c r="H8">
-        <f>AVERAGE(C8:F8)</f>
+        <f t="shared" si="4"/>
         <v>43.930477002543199</v>
       </c>
       <c r="I8">
-        <f>AVERAGE(D8,F8,G8)</f>
+        <f t="shared" si="0"/>
         <v>32.329941308477466</v>
       </c>
       <c r="J8">
-        <f>_xlfn.STDEV.P(D8,F8,G8)</f>
+        <f t="shared" si="1"/>
         <v>2.337231049851805</v>
       </c>
       <c r="K8">
-        <f>_xlfn.STDEV.P(C8:G8)</f>
+        <f t="shared" si="2"/>
         <v>11.600452924666333</v>
       </c>
       <c r="L8" s="4">
-        <f>K8/H8</f>
+        <f t="shared" si="3"/>
         <v>0.26406389632406602</v>
       </c>
       <c r="M8" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N8" t="s">
         <v>466</v>
@@ -13679,7 +13681,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
+      <c r="A9" t="s">
         <v>460</v>
       </c>
       <c r="B9" t="s">
@@ -13704,23 +13706,23 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <f>AVERAGE(D9,F9,G9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J9">
-        <f>_xlfn.STDEV.P(D9,F9,G9)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K9">
-        <f>_xlfn.STDEV.P(C9:G9)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L9" t="e">
-        <f>K9/H9</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M9" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N9" t="s">
         <v>467</v>
@@ -13759,27 +13761,27 @@
         <v>38.655692829940598</v>
       </c>
       <c r="H10">
-        <f>AVERAGE(C10:F10)</f>
+        <f t="shared" ref="H10:H41" si="5">AVERAGE(C10:F10)</f>
         <v>47.539791948168933</v>
       </c>
       <c r="I10">
-        <f>AVERAGE(D10,F10,G10)</f>
+        <f t="shared" si="0"/>
         <v>41.362282891482465</v>
       </c>
       <c r="J10">
-        <f>_xlfn.STDEV.P(D10,F10,G10)</f>
+        <f t="shared" si="1"/>
         <v>2.8087610118691795</v>
       </c>
       <c r="K10">
-        <f>_xlfn.STDEV.P(C10:G10)</f>
+        <f t="shared" si="2"/>
         <v>7.2717368848070576</v>
       </c>
       <c r="L10" s="4">
-        <f>K10/H10</f>
+        <f t="shared" si="3"/>
         <v>0.15296105823801653</v>
       </c>
       <c r="M10" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N10" t="s">
         <v>466</v>
@@ -13820,27 +13822,27 @@
         <v>21.9453529617894</v>
       </c>
       <c r="H11">
-        <f>AVERAGE(C11:F11)</f>
+        <f t="shared" si="5"/>
         <v>39.319612070798009</v>
       </c>
       <c r="I11">
-        <f>AVERAGE(D11,F11,G11)</f>
+        <f t="shared" si="0"/>
         <v>24.4193804149938</v>
       </c>
       <c r="J11">
-        <f>_xlfn.STDEV.P(D11,F11,G11)</f>
+        <f t="shared" si="1"/>
         <v>2.1455535549424152</v>
       </c>
       <c r="K11">
-        <f>_xlfn.STDEV.P(C11:G11)</f>
+        <f t="shared" si="2"/>
         <v>17.654175065529426</v>
       </c>
       <c r="L11" s="4">
-        <f>K11/H11</f>
+        <f t="shared" si="3"/>
         <v>0.44899158805894918</v>
       </c>
       <c r="M11" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N11" t="s">
         <v>466</v>
@@ -13881,27 +13883,27 @@
         <v>31.680387597935201</v>
       </c>
       <c r="H12">
-        <f>AVERAGE(C12:F12)</f>
+        <f t="shared" si="5"/>
         <v>44.284177973095701</v>
       </c>
       <c r="I12">
-        <f>AVERAGE(D12,F12,G12)</f>
+        <f t="shared" si="0"/>
         <v>33.610266496772674</v>
       </c>
       <c r="J12">
-        <f>_xlfn.STDEV.P(D12,F12,G12)</f>
+        <f t="shared" si="1"/>
         <v>3.2768604437237241</v>
       </c>
       <c r="K12">
-        <f>_xlfn.STDEV.P(C12:G12)</f>
+        <f t="shared" si="2"/>
         <v>10.412398316315842</v>
       </c>
       <c r="L12" s="4">
-        <f>K12/H12</f>
+        <f t="shared" si="3"/>
         <v>0.23512682842711374</v>
       </c>
       <c r="M12" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N12" t="s">
         <v>466</v>
@@ -13942,27 +13944,27 @@
         <v>39.304469987386803</v>
       </c>
       <c r="H13">
-        <f>AVERAGE(C13:F13)</f>
+        <f t="shared" si="5"/>
         <v>55.028254497165072</v>
       </c>
       <c r="I13">
-        <f>AVERAGE(D13,F13,G13)</f>
+        <f t="shared" si="0"/>
         <v>42.088465992015699</v>
       </c>
       <c r="J13">
-        <f>_xlfn.STDEV.P(D13,F13,G13)</f>
+        <f t="shared" si="1"/>
         <v>2.2835292053535694</v>
       </c>
       <c r="K13">
-        <f>_xlfn.STDEV.P(C13:G13)</f>
+        <f t="shared" si="2"/>
         <v>12.276181240075342</v>
       </c>
       <c r="L13" s="4">
-        <f>K13/H13</f>
+        <f t="shared" si="3"/>
         <v>0.2230886905690927</v>
       </c>
       <c r="M13" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N13" t="s">
         <v>466</v>
@@ -14003,27 +14005,27 @@
         <v>32.308771113994602</v>
       </c>
       <c r="H14">
-        <f>AVERAGE(C14:F14)</f>
+        <f t="shared" si="5"/>
         <v>54.067311158551718</v>
       </c>
       <c r="I14">
-        <f>AVERAGE(D14,F14,G14)</f>
+        <f t="shared" si="0"/>
         <v>35.7459252494005</v>
       </c>
       <c r="J14">
-        <f>_xlfn.STDEV.P(D14,F14,G14)</f>
+        <f t="shared" si="1"/>
         <v>2.450798412253687</v>
       </c>
       <c r="K14">
-        <f>_xlfn.STDEV.P(C14:G14)</f>
+        <f t="shared" si="2"/>
         <v>17.570104515088595</v>
       </c>
       <c r="L14" s="4">
-        <f>K14/H14</f>
+        <f t="shared" si="3"/>
         <v>0.32496723322460924</v>
       </c>
       <c r="M14" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N14" t="s">
         <v>466</v>
@@ -14064,27 +14066,27 @@
         <v>33.421516319064501</v>
       </c>
       <c r="H15">
-        <f>AVERAGE(C15:F15)</f>
+        <f t="shared" si="5"/>
         <v>53.009261465993376</v>
       </c>
       <c r="I15">
-        <f>AVERAGE(D15,F15,G15)</f>
+        <f t="shared" si="0"/>
         <v>37.095867394345994</v>
       </c>
       <c r="J15">
-        <f>_xlfn.STDEV.P(D15,F15,G15)</f>
+        <f t="shared" si="1"/>
         <v>2.9637649058159066</v>
       </c>
       <c r="K15">
-        <f>_xlfn.STDEV.P(C15:G15)</f>
+        <f t="shared" si="2"/>
         <v>15.923846982311037</v>
       </c>
       <c r="L15" s="4">
-        <f>K15/H15</f>
+        <f t="shared" si="3"/>
         <v>0.30039745021776132</v>
       </c>
       <c r="M15" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N15" t="s">
         <v>466</v>
@@ -14122,27 +14124,27 @@
         <v>29.9416192635553</v>
       </c>
       <c r="H16">
-        <f>AVERAGE(C16:F16)</f>
+        <f t="shared" si="5"/>
         <v>50.981281892195696</v>
       </c>
       <c r="I16">
-        <f>AVERAGE(D16,F16,G16)</f>
+        <f t="shared" si="0"/>
         <v>34.798092277446031</v>
       </c>
       <c r="J16">
-        <f>_xlfn.STDEV.P(D16,F16,G16)</f>
+        <f t="shared" si="1"/>
         <v>3.4589261033301284</v>
       </c>
       <c r="K16">
-        <f>_xlfn.STDEV.P(C16:G16)</f>
+        <f t="shared" si="2"/>
         <v>16.764013083551077</v>
       </c>
       <c r="L16" s="4">
-        <f>K16/H16</f>
+        <f t="shared" si="3"/>
         <v>0.32882682548077202</v>
       </c>
       <c r="M16" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N16" t="s">
         <v>466</v>
@@ -14183,27 +14185,27 @@
         <v>20.352209802182902</v>
       </c>
       <c r="H17">
-        <f>AVERAGE(C17:F17)</f>
+        <f t="shared" si="5"/>
         <v>37.3604415909927</v>
       </c>
       <c r="I17">
-        <f>AVERAGE(D17,F17,G17)</f>
+        <f t="shared" si="0"/>
         <v>22.997958722051234</v>
       </c>
       <c r="J17">
-        <f>_xlfn.STDEV.P(D17,F17,G17)</f>
+        <f t="shared" si="1"/>
         <v>1.895635210562818</v>
       </c>
       <c r="K17">
-        <f>_xlfn.STDEV.P(C17:G17)</f>
+        <f t="shared" si="2"/>
         <v>16.00585174143394</v>
       </c>
       <c r="L17" s="4">
-        <f>K17/H17</f>
+        <f t="shared" si="3"/>
         <v>0.42841709197818534</v>
       </c>
       <c r="M17" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N17" t="s">
         <v>466</v>
@@ -14244,27 +14246,27 @@
         <v>26.959225705586601</v>
       </c>
       <c r="H18">
-        <f>AVERAGE(C18:F18)</f>
+        <f t="shared" si="5"/>
         <v>37.897541350851547</v>
       </c>
       <c r="I18">
-        <f>AVERAGE(D18,F18,G18)</f>
+        <f t="shared" si="0"/>
         <v>27.965183702997603</v>
       </c>
       <c r="J18">
-        <f>_xlfn.STDEV.P(D18,F18,G18)</f>
+        <f t="shared" si="1"/>
         <v>1.2355894903292308</v>
       </c>
       <c r="K18">
-        <f>_xlfn.STDEV.P(C18:G18)</f>
+        <f t="shared" si="2"/>
         <v>9.9747470680035679</v>
       </c>
       <c r="L18" s="4">
-        <f>K18/H18</f>
+        <f t="shared" si="3"/>
         <v>0.26320301297802895</v>
       </c>
       <c r="M18" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N18" t="s">
         <v>466</v>
@@ -14305,27 +14307,27 @@
         <v>23.3457352398263</v>
       </c>
       <c r="H19">
-        <f>AVERAGE(C19:F19)</f>
+        <f t="shared" si="5"/>
         <v>33.147901962236325</v>
       </c>
       <c r="I19">
-        <f>AVERAGE(D19,F19,G19)</f>
+        <f t="shared" si="0"/>
         <v>24.473547696257199</v>
       </c>
       <c r="J19">
-        <f>_xlfn.STDEV.P(D19,F19,G19)</f>
+        <f t="shared" si="1"/>
         <v>0.79993374793040029</v>
       </c>
       <c r="K19">
-        <f>_xlfn.STDEV.P(C19:G19)</f>
+        <f t="shared" si="2"/>
         <v>8.2795313394697612</v>
       </c>
       <c r="L19" s="4">
-        <f>K19/H19</f>
+        <f t="shared" si="3"/>
         <v>0.24977542617635948</v>
       </c>
       <c r="M19" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N19" t="s">
         <v>466</v>
@@ -14366,27 +14368,27 @@
         <v>24.537122060902501</v>
       </c>
       <c r="H20">
-        <f>AVERAGE(C20:F20)</f>
+        <f t="shared" si="5"/>
         <v>35.662045618418077</v>
       </c>
       <c r="I20">
-        <f>AVERAGE(D20,F20,G20)</f>
+        <f t="shared" si="0"/>
         <v>26.69776484485827</v>
       </c>
       <c r="J20">
-        <f>_xlfn.STDEV.P(D20,F20,G20)</f>
+        <f t="shared" si="1"/>
         <v>1.5696013844198631</v>
       </c>
       <c r="K20">
-        <f>_xlfn.STDEV.P(C20:G20)</f>
+        <f t="shared" si="2"/>
         <v>8.4548814845432823</v>
       </c>
       <c r="L20" s="4">
-        <f>K20/H20</f>
+        <f t="shared" si="3"/>
         <v>0.23708346893529464</v>
       </c>
       <c r="M20" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N20" t="s">
         <v>466</v>
@@ -14427,27 +14429,27 @@
         <v>21.4979096286506</v>
       </c>
       <c r="H21">
-        <f>AVERAGE(C21:F21)</f>
+        <f t="shared" si="5"/>
         <v>31.987361288497425</v>
       </c>
       <c r="I21">
-        <f>AVERAGE(D21,F21,G21)</f>
+        <f t="shared" si="0"/>
         <v>21.9975082608801</v>
       </c>
       <c r="J21">
-        <f>_xlfn.STDEV.P(D21,F21,G21)</f>
+        <f t="shared" si="1"/>
         <v>0.43001474281731356</v>
       </c>
       <c r="K21">
-        <f>_xlfn.STDEV.P(C21:G21)</f>
+        <f t="shared" si="2"/>
         <v>11.118331987509753</v>
       </c>
       <c r="L21" s="4">
-        <f>K21/H21</f>
+        <f t="shared" si="3"/>
         <v>0.3475851567508908</v>
       </c>
       <c r="M21" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N21" t="s">
         <v>466</v>
@@ -14488,27 +14490,27 @@
         <v>22.193803373861101</v>
       </c>
       <c r="H22">
-        <f>AVERAGE(C22:F22)</f>
+        <f t="shared" si="5"/>
         <v>40.538678709809169</v>
       </c>
       <c r="I22">
-        <f>AVERAGE(D22,F22,G22)</f>
+        <f t="shared" si="0"/>
         <v>30.644339404365933</v>
       </c>
       <c r="J22">
-        <f>_xlfn.STDEV.P(D22,F22,G22)</f>
+        <f t="shared" si="1"/>
         <v>6.6765458964241482</v>
       </c>
       <c r="K22">
-        <f>_xlfn.STDEV.P(C22:G22)</f>
+        <f t="shared" si="2"/>
         <v>9.6692974776281311</v>
       </c>
       <c r="L22" s="4">
-        <f>K22/H22</f>
+        <f t="shared" si="3"/>
         <v>0.23852029186359361</v>
       </c>
       <c r="M22" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N22" t="s">
         <v>466</v>
@@ -14549,27 +14551,27 @@
         <v>17.653695224930299</v>
       </c>
       <c r="H23">
-        <f>AVERAGE(C23:F23)</f>
+        <f t="shared" si="5"/>
         <v>32.216961135827297</v>
       </c>
       <c r="I23">
-        <f>AVERAGE(D23,F23,G23)</f>
+        <f t="shared" si="0"/>
         <v>21.488819922746501</v>
       </c>
       <c r="J23">
-        <f>_xlfn.STDEV.P(D23,F23,G23)</f>
+        <f t="shared" si="1"/>
         <v>2.7119378791755313</v>
       </c>
       <c r="K23">
-        <f>_xlfn.STDEV.P(C23:G23)</f>
+        <f t="shared" si="2"/>
         <v>12.521782349546291</v>
       </c>
       <c r="L23" s="4">
-        <f>K23/H23</f>
+        <f t="shared" si="3"/>
         <v>0.38867049864679126</v>
       </c>
       <c r="M23" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N23" t="s">
         <v>466</v>
@@ -14610,27 +14612,27 @@
         <v>25.769088486307101</v>
       </c>
       <c r="H24">
-        <f>AVERAGE(C24:F24)</f>
+        <f t="shared" si="5"/>
         <v>34.470016162072952</v>
       </c>
       <c r="I24">
-        <f>AVERAGE(D24,F24,G24)</f>
+        <f t="shared" si="0"/>
         <v>27.896937711532967</v>
       </c>
       <c r="J24">
-        <f>_xlfn.STDEV.P(D24,F24,G24)</f>
+        <f t="shared" si="1"/>
         <v>1.7760201239452371</v>
       </c>
       <c r="K24">
-        <f>_xlfn.STDEV.P(C24:G24)</f>
+        <f t="shared" si="2"/>
         <v>6.1870496077071255</v>
       </c>
       <c r="L24" s="4">
-        <f>K24/H24</f>
+        <f t="shared" si="3"/>
         <v>0.17949076607961328</v>
       </c>
       <c r="M24" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N24" t="s">
         <v>466</v>
@@ -14671,27 +14673,27 @@
         <v>14.8699802070958</v>
       </c>
       <c r="H25">
-        <f>AVERAGE(C25:F25)</f>
+        <f t="shared" si="5"/>
         <v>24.556999985293778</v>
       </c>
       <c r="I25">
-        <f>AVERAGE(D25,F25,G25)</f>
+        <f t="shared" si="0"/>
         <v>15.015536716090301</v>
       </c>
       <c r="J25">
-        <f>_xlfn.STDEV.P(D25,F25,G25)</f>
+        <f t="shared" si="1"/>
         <v>0.5507622276843166</v>
       </c>
       <c r="K25">
-        <f>_xlfn.STDEV.P(C25:G25)</f>
+        <f t="shared" si="2"/>
         <v>14.150444444340691</v>
       </c>
       <c r="L25" s="4">
-        <f>K25/H25</f>
+        <f t="shared" si="3"/>
         <v>0.5762285479828495</v>
       </c>
       <c r="M25" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N25" t="s">
         <v>466</v>
@@ -14732,27 +14734,27 @@
         <v>30.712356200963502</v>
       </c>
       <c r="H26">
-        <f>AVERAGE(C26:F26)</f>
+        <f t="shared" si="5"/>
         <v>35.133921411357079</v>
       </c>
       <c r="I26">
-        <f>AVERAGE(D26,F26,G26)</f>
+        <f t="shared" si="0"/>
         <v>29.765880615463931</v>
       </c>
       <c r="J26">
-        <f>_xlfn.STDEV.P(D26,F26,G26)</f>
+        <f t="shared" si="1"/>
         <v>1.1315592043518403</v>
       </c>
       <c r="K26">
-        <f>_xlfn.STDEV.P(C26:G26)</f>
+        <f t="shared" si="2"/>
         <v>7.2725350950834384</v>
       </c>
       <c r="L26" s="4">
-        <f>K26/H26</f>
+        <f t="shared" si="3"/>
         <v>0.20699468783841998</v>
       </c>
       <c r="M26" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N26" t="s">
         <v>466</v>
@@ -14793,27 +14795,27 @@
         <v>29.9620055057425</v>
       </c>
       <c r="H27">
-        <f>AVERAGE(C27:F27)</f>
+        <f t="shared" si="5"/>
         <v>45.993618886234273</v>
       </c>
       <c r="I27">
-        <f>AVERAGE(D27,F27,G27)</f>
+        <f t="shared" si="0"/>
         <v>31.839250350226532</v>
       </c>
       <c r="J27">
-        <f>_xlfn.STDEV.P(D27,F27,G27)</f>
+        <f t="shared" si="1"/>
         <v>1.3434111734858469</v>
       </c>
       <c r="K27">
-        <f>_xlfn.STDEV.P(C27:G27)</f>
+        <f t="shared" si="2"/>
         <v>14.944683511226884</v>
       </c>
       <c r="L27" s="4">
-        <f>K27/H27</f>
+        <f t="shared" si="3"/>
         <v>0.32492949833307799</v>
       </c>
       <c r="M27" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N27" t="s">
         <v>466</v>
@@ -14854,27 +14856,27 @@
         <v>14.2301417533457</v>
       </c>
       <c r="H28">
-        <f>AVERAGE(C28:F28)</f>
+        <f t="shared" si="5"/>
         <v>30.159978787847503</v>
       </c>
       <c r="I28">
-        <f>AVERAGE(D28,F28,G28)</f>
+        <f t="shared" si="0"/>
         <v>15.361618968245233</v>
       </c>
       <c r="J28">
-        <f>_xlfn.STDEV.P(D28,F28,G28)</f>
+        <f t="shared" si="1"/>
         <v>1.3901668822288946</v>
       </c>
       <c r="K28">
-        <f>_xlfn.STDEV.P(C28:G28)</f>
+        <f t="shared" si="2"/>
         <v>18.726580116927192</v>
       </c>
       <c r="L28" s="4">
-        <f>K28/H28</f>
+        <f t="shared" si="3"/>
         <v>0.62090826550822298</v>
       </c>
       <c r="M28" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N28" t="s">
         <v>466</v>
@@ -14915,27 +14917,27 @@
         <v>12.9018004593177</v>
       </c>
       <c r="H29">
-        <f>AVERAGE(C29:F29)</f>
+        <f t="shared" si="5"/>
         <v>20.24790800327975</v>
       </c>
       <c r="I29">
-        <f>AVERAGE(D29,F29,G29)</f>
+        <f t="shared" si="0"/>
         <v>13.630844157478899</v>
       </c>
       <c r="J29">
-        <f>_xlfn.STDEV.P(D29,F29,G29)</f>
+        <f t="shared" si="1"/>
         <v>0.64744337877436209</v>
       </c>
       <c r="K29">
-        <f>_xlfn.STDEV.P(C29:G29)</f>
+        <f t="shared" si="2"/>
         <v>8.9885917255728103</v>
       </c>
       <c r="L29" s="4">
-        <f>K29/H29</f>
+        <f t="shared" si="3"/>
         <v>0.44392693428461055</v>
       </c>
       <c r="M29" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N29" t="s">
         <v>466</v>
@@ -14976,27 +14978,27 @@
         <v>10.4689189958616</v>
       </c>
       <c r="H30">
-        <f>AVERAGE(C30:F30)</f>
+        <f t="shared" si="5"/>
         <v>20.147831354696475</v>
       </c>
       <c r="I30">
-        <f>AVERAGE(D30,F30,G30)</f>
+        <f t="shared" si="0"/>
         <v>12.9436148048825</v>
       </c>
       <c r="J30">
-        <f>_xlfn.STDEV.P(D30,F30,G30)</f>
+        <f t="shared" si="1"/>
         <v>1.7932794989538992</v>
       </c>
       <c r="K30">
-        <f>_xlfn.STDEV.P(C30:G30)</f>
+        <f t="shared" si="2"/>
         <v>7.8374946793647933</v>
       </c>
       <c r="L30" s="4">
-        <f>K30/H30</f>
+        <f t="shared" si="3"/>
         <v>0.38899941841819452</v>
       </c>
       <c r="M30" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N30" t="s">
         <v>466</v>
@@ -15037,27 +15039,27 @@
         <v>9.2213284432397593</v>
       </c>
       <c r="H31">
-        <f>AVERAGE(C31:F31)</f>
+        <f t="shared" si="5"/>
         <v>12.089359845064109</v>
       </c>
       <c r="I31">
-        <f>AVERAGE(D31,F31,G31)</f>
+        <f t="shared" si="0"/>
         <v>8.7736796078320669</v>
       </c>
       <c r="J31">
-        <f>_xlfn.STDEV.P(D31,F31,G31)</f>
+        <f t="shared" si="1"/>
         <v>1.4657820377610455</v>
       </c>
       <c r="K31">
-        <f>_xlfn.STDEV.P(C31:G31)</f>
+        <f t="shared" si="2"/>
         <v>8.1108597001947764</v>
       </c>
       <c r="L31" s="4">
-        <f>K31/H31</f>
+        <f t="shared" si="3"/>
         <v>0.6709089483763121</v>
       </c>
       <c r="M31" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N31" t="s">
         <v>466</v>
@@ -15098,27 +15100,27 @@
         <v>6.8417408766984602</v>
       </c>
       <c r="H32">
-        <f>AVERAGE(C32:F32)</f>
+        <f t="shared" si="5"/>
         <v>8.4785455090424904</v>
       </c>
       <c r="I32">
-        <f>AVERAGE(D32,F32,G32)</f>
+        <f t="shared" si="0"/>
         <v>6.6323909709561404</v>
       </c>
       <c r="J32">
-        <f>_xlfn.STDEV.P(D32,F32,G32)</f>
+        <f t="shared" si="1"/>
         <v>3.531037998489202</v>
       </c>
       <c r="K32">
-        <f>_xlfn.STDEV.P(C32:G32)</f>
+        <f t="shared" si="2"/>
         <v>3.9133635088437897</v>
       </c>
       <c r="L32" s="4">
-        <f>K32/H32</f>
+        <f t="shared" si="3"/>
         <v>0.46156071282157196</v>
       </c>
       <c r="M32" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N32" t="s">
         <v>466</v>
@@ -15159,27 +15161,27 @@
         <v>9.0646765683026</v>
       </c>
       <c r="H33">
-        <f>AVERAGE(C33:F33)</f>
+        <f t="shared" si="5"/>
         <v>7.8730615303211522</v>
       </c>
       <c r="I33">
-        <f>AVERAGE(D33,F33,G33)</f>
+        <f t="shared" si="0"/>
         <v>8.1607478965290685</v>
       </c>
       <c r="J33">
-        <f>_xlfn.STDEV.P(D33,F33,G33)</f>
+        <f t="shared" si="1"/>
         <v>2.2286642648816466</v>
       </c>
       <c r="K33">
-        <f>_xlfn.STDEV.P(C33:G33)</f>
+        <f t="shared" si="2"/>
         <v>3.1588768316318512</v>
       </c>
       <c r="L33" s="4">
-        <f>K33/H33</f>
+        <f t="shared" si="3"/>
         <v>0.4012259804481671</v>
       </c>
       <c r="M33" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N33" t="s">
         <v>466</v>
@@ -15220,27 +15222,27 @@
         <v>13.7978945484861</v>
       </c>
       <c r="H34">
-        <f>AVERAGE(C34:F34)</f>
+        <f t="shared" si="5"/>
         <v>18.752405463820502</v>
       </c>
       <c r="I34">
-        <f>AVERAGE(D34,F34,G34)</f>
+        <f t="shared" ref="I34:I65" si="6">AVERAGE(D34,F34,G34)</f>
         <v>16.857045467922699</v>
       </c>
       <c r="J34">
-        <f>_xlfn.STDEV.P(D34,F34,G34)</f>
+        <f t="shared" ref="J34:J65" si="7">_xlfn.STDEV.P(D34,F34,G34)</f>
         <v>2.300297125915217</v>
       </c>
       <c r="K34">
-        <f>_xlfn.STDEV.P(C34:G34)</f>
+        <f t="shared" ref="K34:K65" si="8">_xlfn.STDEV.P(C34:G34)</f>
         <v>2.9811926905724477</v>
       </c>
       <c r="L34" s="4">
-        <f>K34/H34</f>
+        <f t="shared" ref="L34:L65" si="9">K34/H34</f>
         <v>0.15897654817266721</v>
       </c>
       <c r="M34" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N34" t="s">
         <v>466</v>
@@ -15281,27 +15283,27 @@
         <v>14.263203360011801</v>
       </c>
       <c r="H35">
-        <f>AVERAGE(C35:F35)</f>
+        <f t="shared" si="5"/>
         <v>23.619150399342846</v>
       </c>
       <c r="I35">
-        <f>AVERAGE(D35,F35,G35)</f>
+        <f t="shared" si="6"/>
         <v>16.973434985794398</v>
       </c>
       <c r="J35">
-        <f>_xlfn.STDEV.P(D35,F35,G35)</f>
+        <f t="shared" si="7"/>
         <v>2.2042914238059175</v>
       </c>
       <c r="K35">
-        <f>_xlfn.STDEV.P(C35:G35)</f>
+        <f t="shared" si="8"/>
         <v>7.1594075058961941</v>
       </c>
       <c r="L35" s="4">
-        <f>K35/H35</f>
+        <f t="shared" si="9"/>
         <v>0.30311875680741629</v>
       </c>
       <c r="M35" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N35" t="s">
         <v>466</v>
@@ -15342,27 +15344,27 @@
         <v>16.879975707983</v>
       </c>
       <c r="H36">
-        <f>AVERAGE(C36:F36)</f>
+        <f t="shared" si="5"/>
         <v>26.738979933596724</v>
       </c>
       <c r="I36">
-        <f>AVERAGE(D36,F36,G36)</f>
+        <f t="shared" si="6"/>
         <v>19.835345147456632</v>
       </c>
       <c r="J36">
-        <f>_xlfn.STDEV.P(D36,F36,G36)</f>
+        <f t="shared" si="7"/>
         <v>2.2848312935788049</v>
       </c>
       <c r="K36">
-        <f>_xlfn.STDEV.P(C36:G36)</f>
+        <f t="shared" si="8"/>
         <v>6.590294975681017</v>
       </c>
       <c r="L36" s="4">
-        <f>K36/H36</f>
+        <f t="shared" si="9"/>
         <v>0.2464677034070589</v>
       </c>
       <c r="M36" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N36" t="s">
         <v>466</v>
@@ -15403,27 +15405,27 @@
         <v>16.493774392662601</v>
       </c>
       <c r="H37">
-        <f>AVERAGE(C37:F37)</f>
+        <f t="shared" si="5"/>
         <v>24.857484028944903</v>
       </c>
       <c r="I37">
-        <f>AVERAGE(D37,F37,G37)</f>
+        <f t="shared" si="6"/>
         <v>17.512886836147402</v>
       </c>
       <c r="J37">
-        <f>_xlfn.STDEV.P(D37,F37,G37)</f>
+        <f t="shared" si="7"/>
         <v>1.3317656359780452</v>
       </c>
       <c r="K37">
-        <f>_xlfn.STDEV.P(C37:G37)</f>
+        <f t="shared" si="8"/>
         <v>8.108661441289895</v>
       </c>
       <c r="L37" s="4">
-        <f>K37/H37</f>
+        <f t="shared" si="9"/>
         <v>0.32620604047649765</v>
       </c>
       <c r="M37" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N37" t="s">
         <v>466</v>
@@ -15464,27 +15466,27 @@
         <v>30.019442833052</v>
       </c>
       <c r="H38">
-        <f>AVERAGE(C38:F38)</f>
+        <f t="shared" si="5"/>
         <v>38.501347714413654</v>
       </c>
       <c r="I38">
-        <f>AVERAGE(D38,F38,G38)</f>
+        <f t="shared" si="6"/>
         <v>31.353201230235531</v>
       </c>
       <c r="J38">
-        <f>_xlfn.STDEV.P(D38,F38,G38)</f>
+        <f t="shared" si="7"/>
         <v>1.634683784384005</v>
       </c>
       <c r="K38">
-        <f>_xlfn.STDEV.P(C38:G38)</f>
+        <f t="shared" si="8"/>
         <v>6.8953160836348237</v>
       </c>
       <c r="L38" s="4">
-        <f>K38/H38</f>
+        <f t="shared" si="9"/>
         <v>0.17909284980830531</v>
       </c>
       <c r="M38" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N38" t="s">
         <v>466</v>
@@ -15525,27 +15527,27 @@
         <v>18.640819524197401</v>
       </c>
       <c r="H39">
-        <f>AVERAGE(C39:F39)</f>
+        <f t="shared" si="5"/>
         <v>35.563188841650174</v>
       </c>
       <c r="I39">
-        <f>AVERAGE(D39,F39,G39)</f>
+        <f t="shared" si="6"/>
         <v>20.646774963599366</v>
       </c>
       <c r="J39">
-        <f>_xlfn.STDEV.P(D39,F39,G39)</f>
+        <f t="shared" si="7"/>
         <v>1.4210040912819224</v>
       </c>
       <c r="K39">
-        <f>_xlfn.STDEV.P(C39:G39)</f>
+        <f t="shared" si="8"/>
         <v>18.021399772958752</v>
       </c>
       <c r="L39" s="4">
-        <f>K39/H39</f>
+        <f t="shared" si="9"/>
         <v>0.50674307788318507</v>
       </c>
       <c r="M39" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N39" t="s">
         <v>466</v>
@@ -15586,27 +15588,27 @@
         <v>17.989919770028798</v>
       </c>
       <c r="H40">
-        <f>AVERAGE(C40:F40)</f>
+        <f t="shared" si="5"/>
         <v>29.474180347480729</v>
       </c>
       <c r="I40">
-        <f>AVERAGE(D40,F40,G40)</f>
+        <f t="shared" si="6"/>
         <v>19.972770386650566</v>
       </c>
       <c r="J40">
-        <f>_xlfn.STDEV.P(D40,F40,G40)</f>
+        <f t="shared" si="7"/>
         <v>1.9858607362875469</v>
       </c>
       <c r="K40">
-        <f>_xlfn.STDEV.P(C40:G40)</f>
+        <f t="shared" si="8"/>
         <v>10.499087551927412</v>
       </c>
       <c r="L40" s="4">
-        <f>K40/H40</f>
+        <f t="shared" si="9"/>
         <v>0.35621304572850687</v>
       </c>
       <c r="M40" t="s">
-        <v>363</v>
+        <v>472</v>
       </c>
       <c r="N40" t="s">
         <v>466</v>
@@ -15647,27 +15649,27 @@
         <v>17.456148279238199</v>
       </c>
       <c r="H41">
-        <f>AVERAGE(C41:F41)</f>
+        <f t="shared" si="5"/>
         <v>27.511929704452871</v>
       </c>
       <c r="I41">
-        <f>AVERAGE(D41,F41,G41)</f>
+        <f t="shared" si="6"/>
         <v>17.766482365683235</v>
       </c>
       <c r="J41">
-        <f>_xlfn.STDEV.P(D41,F41,G41)</f>
+        <f t="shared" si="7"/>
         <v>0.33842452036444792</v>
       </c>
       <c r="K41">
-        <f>_xlfn.STDEV.P(C41:G41)</f>
+        <f t="shared" si="8"/>
         <v>10.781185436861103</v>
       </c>
       <c r="L41" s="4">
-        <f>K41/H41</f>
+        <f t="shared" si="9"/>
         <v>0.3918731093266839</v>
       </c>
       <c r="M41" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N41" t="s">
         <v>466</v>
@@ -15708,27 +15710,27 @@
         <v>23.708214576376001</v>
       </c>
       <c r="H42">
-        <f>AVERAGE(C42:F42)</f>
+        <f t="shared" ref="H42:H73" si="10">AVERAGE(C42:F42)</f>
         <v>32.67631265004232</v>
       </c>
       <c r="I42">
-        <f>AVERAGE(D42,F42,G42)</f>
+        <f t="shared" si="6"/>
         <v>27.043151725515099</v>
       </c>
       <c r="J42">
-        <f>_xlfn.STDEV.P(D42,F42,G42)</f>
+        <f t="shared" si="7"/>
         <v>3.8213254449905687</v>
       </c>
       <c r="K42">
-        <f>_xlfn.STDEV.P(C42:G42)</f>
+        <f t="shared" si="8"/>
         <v>6.0979489403922313</v>
       </c>
       <c r="L42" s="4">
-        <f>K42/H42</f>
+        <f t="shared" si="9"/>
         <v>0.18661680115808091</v>
       </c>
       <c r="M42" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N42" t="s">
         <v>466</v>
@@ -15769,27 +15771,27 @@
         <v>23.148221757381901</v>
       </c>
       <c r="H43">
-        <f>AVERAGE(C43:F43)</f>
+        <f t="shared" si="10"/>
         <v>34.268387254439176</v>
       </c>
       <c r="I43">
-        <f>AVERAGE(D43,F43,G43)</f>
+        <f t="shared" si="6"/>
         <v>25.8551369250462</v>
       </c>
       <c r="J43">
-        <f>_xlfn.STDEV.P(D43,F43,G43)</f>
+        <f t="shared" si="7"/>
         <v>2.4399560149525517</v>
       </c>
       <c r="K43">
-        <f>_xlfn.STDEV.P(C43:G43)</f>
+        <f t="shared" si="8"/>
         <v>8.0078953225521179</v>
       </c>
       <c r="L43" s="4">
-        <f>K43/H43</f>
+        <f t="shared" si="9"/>
         <v>0.23368170970796892</v>
       </c>
       <c r="M43" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N43" t="s">
         <v>466</v>
@@ -15830,27 +15832,27 @@
         <v>5.8717234707231301</v>
       </c>
       <c r="H44">
-        <f>AVERAGE(C44:F44)</f>
+        <f t="shared" si="10"/>
         <v>14.813175358987058</v>
       </c>
       <c r="I44">
-        <f>AVERAGE(D44,F44,G44)</f>
+        <f t="shared" si="6"/>
         <v>6.1211643022237867</v>
       </c>
       <c r="J44">
-        <f>_xlfn.STDEV.P(D44,F44,G44)</f>
+        <f t="shared" si="7"/>
         <v>0.5422902613262679</v>
       </c>
       <c r="K44">
-        <f>_xlfn.STDEV.P(C44:G44)</f>
+        <f t="shared" si="8"/>
         <v>15.122643326505409</v>
       </c>
       <c r="L44" s="4">
-        <f>K44/H44</f>
+        <f t="shared" si="9"/>
         <v>1.0208913997180624</v>
       </c>
       <c r="M44" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N44" t="s">
         <v>466</v>
@@ -15891,27 +15893,27 @@
         <v>6.3098615913942</v>
       </c>
       <c r="H45">
-        <f>AVERAGE(C45:F45)</f>
+        <f t="shared" si="10"/>
         <v>7.4906746425785222</v>
       </c>
       <c r="I45">
-        <f>AVERAGE(D45,F45,G45)</f>
+        <f t="shared" si="6"/>
         <v>5.8855923872360973</v>
       </c>
       <c r="J45">
-        <f>_xlfn.STDEV.P(D45,F45,G45)</f>
+        <f t="shared" si="7"/>
         <v>0.36573971969646929</v>
       </c>
       <c r="K45">
-        <f>_xlfn.STDEV.P(C45:G45)</f>
+        <f t="shared" si="8"/>
         <v>3.5844345637247987</v>
       </c>
       <c r="L45" s="4">
-        <f>K45/H45</f>
+        <f t="shared" si="9"/>
         <v>0.4785195906587828</v>
       </c>
       <c r="M45" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N45" t="s">
         <v>466</v>
@@ -15952,27 +15954,27 @@
         <v>27.602967991351601</v>
       </c>
       <c r="H46">
-        <f>AVERAGE(C46:F46)</f>
+        <f t="shared" si="10"/>
         <v>29.099845914583575</v>
       </c>
       <c r="I46">
-        <f>AVERAGE(D46,F46,G46)</f>
+        <f t="shared" si="6"/>
         <v>31.723802883228633</v>
       </c>
       <c r="J46">
-        <f>_xlfn.STDEV.P(D46,F46,G46)</f>
+        <f t="shared" si="7"/>
         <v>3.929063695759949</v>
       </c>
       <c r="K46">
-        <f>_xlfn.STDEV.P(C46:G46)</f>
+        <f t="shared" si="8"/>
         <v>13.235230752076545</v>
       </c>
       <c r="L46" s="4">
-        <f>K46/H46</f>
+        <f t="shared" si="9"/>
         <v>0.45482133448148682</v>
       </c>
       <c r="M46" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N46" t="s">
         <v>466</v>
@@ -16013,27 +16015,27 @@
         <v>22.026093065876498</v>
       </c>
       <c r="H47">
-        <f>AVERAGE(C47:F47)</f>
+        <f t="shared" si="10"/>
         <v>36.370009791021602</v>
       </c>
       <c r="I47">
-        <f>AVERAGE(D47,F47,G47)</f>
+        <f t="shared" si="6"/>
         <v>25.8455140766543</v>
       </c>
       <c r="J47">
-        <f>_xlfn.STDEV.P(D47,F47,G47)</f>
+        <f t="shared" si="7"/>
         <v>2.74019660702514</v>
       </c>
       <c r="K47">
-        <f>_xlfn.STDEV.P(C47:G47)</f>
+        <f t="shared" si="8"/>
         <v>11.254445055557376</v>
       </c>
       <c r="L47" s="4">
-        <f>K47/H47</f>
+        <f t="shared" si="9"/>
         <v>0.30944300318378465</v>
       </c>
       <c r="M47" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N47" t="s">
         <v>466</v>
@@ -16074,27 +16076,27 @@
         <v>23.0535027186436</v>
       </c>
       <c r="H48">
-        <f>AVERAGE(C48:F48)</f>
+        <f t="shared" si="10"/>
         <v>35.455263630365778</v>
       </c>
       <c r="I48">
-        <f>AVERAGE(D48,F48,G48)</f>
+        <f t="shared" si="6"/>
         <v>26.293165746702233</v>
       </c>
       <c r="J48">
-        <f>_xlfn.STDEV.P(D48,F48,G48)</f>
+        <f t="shared" si="7"/>
         <v>2.8091673039935978</v>
       </c>
       <c r="K48">
-        <f>_xlfn.STDEV.P(C48:G48)</f>
+        <f t="shared" si="8"/>
         <v>8.8424783775873887</v>
       </c>
       <c r="L48" s="4">
-        <f>K48/H48</f>
+        <f t="shared" si="9"/>
         <v>0.24939818442117628</v>
       </c>
       <c r="M48" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N48" t="s">
         <v>466</v>
@@ -16135,27 +16137,27 @@
         <v>31.4075696138237</v>
       </c>
       <c r="H49">
-        <f>AVERAGE(C49:F49)</f>
+        <f t="shared" si="10"/>
         <v>42.327852855389494</v>
       </c>
       <c r="I49">
-        <f>AVERAGE(D49,F49,G49)</f>
+        <f t="shared" si="6"/>
         <v>34.285657011793901</v>
       </c>
       <c r="J49">
-        <f>_xlfn.STDEV.P(D49,F49,G49)</f>
+        <f t="shared" si="7"/>
         <v>2.0989394974942526</v>
       </c>
       <c r="K49">
-        <f>_xlfn.STDEV.P(C49:G49)</f>
+        <f t="shared" si="8"/>
         <v>7.3939077196467489</v>
       </c>
       <c r="L49" s="4">
-        <f>K49/H49</f>
+        <f t="shared" si="9"/>
         <v>0.17468185180352946</v>
       </c>
       <c r="M49" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N49" t="s">
         <v>466</v>
@@ -16196,27 +16198,27 @@
         <v>39.787619568243699</v>
       </c>
       <c r="H50">
-        <f>AVERAGE(C50:F50)</f>
+        <f t="shared" si="10"/>
         <v>58.034199334462848</v>
       </c>
       <c r="I50">
-        <f>AVERAGE(D50,F50,G50)</f>
+        <f t="shared" si="6"/>
         <v>44.122515635365033</v>
       </c>
       <c r="J50">
-        <f>_xlfn.STDEV.P(D50,F50,G50)</f>
+        <f t="shared" si="7"/>
         <v>3.8796149910365729</v>
       </c>
       <c r="K50">
-        <f>_xlfn.STDEV.P(C50:G50)</f>
+        <f t="shared" si="8"/>
         <v>12.982823542956009</v>
       </c>
       <c r="L50" s="4">
-        <f>K50/H50</f>
+        <f t="shared" si="9"/>
         <v>0.22370987610483548</v>
       </c>
       <c r="M50" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N50" t="s">
         <v>466</v>
@@ -16257,27 +16259,27 @@
         <v>31.8451363658838</v>
       </c>
       <c r="H51">
-        <f>AVERAGE(C51:F51)</f>
+        <f t="shared" si="10"/>
         <v>50.290208123248846</v>
       </c>
       <c r="I51">
-        <f>AVERAGE(D51,F51,G51)</f>
+        <f t="shared" si="6"/>
         <v>33.189169619626398</v>
       </c>
       <c r="J51">
-        <f>_xlfn.STDEV.P(D51,F51,G51)</f>
+        <f t="shared" si="7"/>
         <v>2.8322462440676626</v>
       </c>
       <c r="K51">
-        <f>_xlfn.STDEV.P(C51:G51)</f>
+        <f t="shared" si="8"/>
         <v>19.325016268944783</v>
       </c>
       <c r="L51" s="4">
-        <f>K51/H51</f>
+        <f t="shared" si="9"/>
         <v>0.3842699601000647</v>
       </c>
       <c r="M51" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N51" t="s">
         <v>466</v>
@@ -16318,27 +16320,27 @@
         <v>18.843433209128801</v>
       </c>
       <c r="H52">
-        <f>AVERAGE(C52:F52)</f>
+        <f t="shared" si="10"/>
         <v>36.644594473612351</v>
       </c>
       <c r="I52">
-        <f>AVERAGE(D52,F52,G52)</f>
+        <f t="shared" si="6"/>
         <v>21.69495703452607</v>
       </c>
       <c r="J52">
-        <f>_xlfn.STDEV.P(D52,F52,G52)</f>
+        <f t="shared" si="7"/>
         <v>2.2171449827478065</v>
       </c>
       <c r="K52">
-        <f>_xlfn.STDEV.P(C52:G52)</f>
+        <f t="shared" si="8"/>
         <v>17.695736694760047</v>
       </c>
       <c r="L52" s="4">
-        <f>K52/H52</f>
+        <f t="shared" si="9"/>
         <v>0.48290169256758148</v>
       </c>
       <c r="M52" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N52" t="s">
         <v>466</v>
@@ -16379,27 +16381,27 @@
         <v>23.646202186609099</v>
       </c>
       <c r="H53">
-        <f>AVERAGE(C53:F53)</f>
+        <f t="shared" si="10"/>
         <v>36.967939845219419</v>
       </c>
       <c r="I53">
-        <f>AVERAGE(D53,F53,G53)</f>
+        <f t="shared" si="6"/>
         <v>27.224550522495601</v>
       </c>
       <c r="J53">
-        <f>_xlfn.STDEV.P(D53,F53,G53)</f>
+        <f t="shared" si="7"/>
         <v>2.5307050327955287</v>
       </c>
       <c r="K53">
-        <f>_xlfn.STDEV.P(C53:G53)</f>
+        <f t="shared" si="8"/>
         <v>9.015738925799953</v>
       </c>
       <c r="L53" s="4">
-        <f>K53/H53</f>
+        <f t="shared" si="9"/>
         <v>0.24387993930816354</v>
       </c>
       <c r="M53" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N53" t="s">
         <v>466</v>
@@ -16440,27 +16442,27 @@
         <v>29.408440648920902</v>
       </c>
       <c r="H54">
-        <f>AVERAGE(C54:F54)</f>
+        <f t="shared" si="10"/>
         <v>37.625643265141974</v>
       </c>
       <c r="I54">
-        <f>AVERAGE(D54,F54,G54)</f>
+        <f t="shared" si="6"/>
         <v>28.766131236496268</v>
       </c>
       <c r="J54">
-        <f>_xlfn.STDEV.P(D54,F54,G54)</f>
+        <f t="shared" si="7"/>
         <v>1.7529311691365521</v>
       </c>
       <c r="K54">
-        <f>_xlfn.STDEV.P(C54:G54)</f>
+        <f t="shared" si="8"/>
         <v>10.001991437218861</v>
       </c>
       <c r="L54" s="4">
-        <f>K54/H54</f>
+        <f t="shared" si="9"/>
         <v>0.26582911464759296</v>
       </c>
       <c r="M54" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N54" t="s">
         <v>466</v>
@@ -16501,27 +16503,27 @@
         <v>23.581866196506699</v>
       </c>
       <c r="H55">
-        <f>AVERAGE(C55:F55)</f>
+        <f t="shared" si="10"/>
         <v>34.472022204390804</v>
       </c>
       <c r="I55">
-        <f>AVERAGE(D55,F55,G55)</f>
+        <f t="shared" si="6"/>
         <v>26.845448338023299</v>
       </c>
       <c r="J55">
-        <f>_xlfn.STDEV.P(D55,F55,G55)</f>
+        <f t="shared" si="7"/>
         <v>2.63576879361873</v>
       </c>
       <c r="K55">
-        <f>_xlfn.STDEV.P(C55:G55)</f>
+        <f t="shared" si="8"/>
         <v>7.1176381739397883</v>
       </c>
       <c r="L55" s="4">
-        <f>K55/H55</f>
+        <f t="shared" si="9"/>
         <v>0.20647579453674156</v>
       </c>
       <c r="M55" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N55" t="s">
         <v>466</v>
@@ -16562,27 +16564,27 @@
         <v>22.705826279454701</v>
       </c>
       <c r="H56">
-        <f>AVERAGE(C56:F56)</f>
+        <f t="shared" si="10"/>
         <v>35.919172887187848</v>
       </c>
       <c r="I56">
-        <f>AVERAGE(D56,F56,G56)</f>
+        <f t="shared" si="6"/>
         <v>27.069765942735369</v>
       </c>
       <c r="J56">
-        <f>_xlfn.STDEV.P(D56,F56,G56)</f>
+        <f t="shared" si="7"/>
         <v>3.9643253613659457</v>
       </c>
       <c r="K56">
-        <f>_xlfn.STDEV.P(C56:G56)</f>
+        <f t="shared" si="8"/>
         <v>8.3157324423777705</v>
       </c>
       <c r="L56" s="4">
-        <f>K56/H56</f>
+        <f t="shared" si="9"/>
         <v>0.23151235883117849</v>
       </c>
       <c r="M56" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N56" t="s">
         <v>466</v>
@@ -16623,27 +16625,27 @@
         <v>25.5368184106771</v>
       </c>
       <c r="H57">
-        <f>AVERAGE(C57:F57)</f>
+        <f t="shared" si="10"/>
         <v>35.253224369029596</v>
       </c>
       <c r="I57">
-        <f>AVERAGE(D57,F57,G57)</f>
+        <f t="shared" si="6"/>
         <v>27.969178628931832</v>
       </c>
       <c r="J57">
-        <f>_xlfn.STDEV.P(D57,F57,G57)</f>
+        <f t="shared" si="7"/>
         <v>1.8270269352118897</v>
       </c>
       <c r="K57">
-        <f>_xlfn.STDEV.P(C57:G57)</f>
+        <f t="shared" si="8"/>
         <v>6.7854063016418227</v>
       </c>
       <c r="L57" s="4">
-        <f>K57/H57</f>
+        <f t="shared" si="9"/>
         <v>0.19247618971281641</v>
       </c>
       <c r="M57" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N57" t="s">
         <v>466</v>
@@ -16684,27 +16686,27 @@
         <v>24.113670224242401</v>
       </c>
       <c r="H58">
-        <f>AVERAGE(C58:F58)</f>
+        <f t="shared" si="10"/>
         <v>40.582837617918727</v>
       </c>
       <c r="I58">
-        <f>AVERAGE(D58,F58,G58)</f>
+        <f t="shared" si="6"/>
         <v>30.411073565305767</v>
       </c>
       <c r="J58">
-        <f>_xlfn.STDEV.P(D58,F58,G58)</f>
+        <f t="shared" si="7"/>
         <v>4.5104406693605759</v>
       </c>
       <c r="K58">
-        <f>_xlfn.STDEV.P(C58:G58)</f>
+        <f t="shared" si="8"/>
         <v>9.6515564850294915</v>
       </c>
       <c r="L58" s="4">
-        <f>K58/H58</f>
+        <f t="shared" si="9"/>
         <v>0.23782359863293531</v>
       </c>
       <c r="M58" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N58" t="s">
         <v>466</v>
@@ -16745,27 +16747,27 @@
         <v>23.701256363127701</v>
       </c>
       <c r="H59">
-        <f>AVERAGE(C59:F59)</f>
+        <f t="shared" si="10"/>
         <v>40.378692160732953</v>
       </c>
       <c r="I59">
-        <f>AVERAGE(D59,F59,G59)</f>
+        <f t="shared" si="6"/>
         <v>28.9479416686865</v>
       </c>
       <c r="J59">
-        <f>_xlfn.STDEV.P(D59,F59,G59)</f>
+        <f t="shared" si="7"/>
         <v>3.7220462868130197</v>
       </c>
       <c r="K59">
-        <f>_xlfn.STDEV.P(C59:G59)</f>
+        <f t="shared" si="8"/>
         <v>10.802769147994534</v>
       </c>
       <c r="L59" s="4">
-        <f>K59/H59</f>
+        <f t="shared" si="9"/>
         <v>0.26753638045017952</v>
       </c>
       <c r="M59" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N59" t="s">
         <v>466</v>
@@ -16806,27 +16808,27 @@
         <v>29.8368526732785</v>
       </c>
       <c r="H60">
-        <f>AVERAGE(C60:F60)</f>
+        <f t="shared" si="10"/>
         <v>41.114926390269972</v>
       </c>
       <c r="I60">
-        <f>AVERAGE(D60,F60,G60)</f>
+        <f t="shared" si="6"/>
         <v>31.140349411452799</v>
       </c>
       <c r="J60">
-        <f>_xlfn.STDEV.P(D60,F60,G60)</f>
+        <f t="shared" si="7"/>
         <v>2.3270484634431354</v>
       </c>
       <c r="K60">
-        <f>_xlfn.STDEV.P(C60:G60)</f>
+        <f t="shared" si="8"/>
         <v>9.9349694563552866</v>
       </c>
       <c r="L60" s="4">
-        <f>K60/H60</f>
+        <f t="shared" si="9"/>
         <v>0.24163899412225243</v>
       </c>
       <c r="M60" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N60" t="s">
         <v>466</v>
@@ -16867,27 +16869,27 @@
         <v>16.277300312684499</v>
       </c>
       <c r="H61">
-        <f>AVERAGE(C61:F61)</f>
+        <f t="shared" si="10"/>
         <v>26.796477972476296</v>
       </c>
       <c r="I61">
-        <f>AVERAGE(D61,F61,G61)</f>
+        <f t="shared" si="6"/>
         <v>14.8650340675299</v>
       </c>
       <c r="J61">
-        <f>_xlfn.STDEV.P(D61,F61,G61)</f>
+        <f t="shared" si="7"/>
         <v>1.4315409585927557</v>
       </c>
       <c r="K61">
-        <f>_xlfn.STDEV.P(C61:G61)</f>
+        <f t="shared" si="8"/>
         <v>15.86255897192266</v>
       </c>
       <c r="L61" s="4">
-        <f>K61/H61</f>
+        <f t="shared" si="9"/>
         <v>0.59196432412557021</v>
       </c>
       <c r="M61" t="s">
-        <v>363</v>
+        <v>471</v>
       </c>
       <c r="N61" t="s">
         <v>466</v>
@@ -16928,23 +16930,23 @@
         <v>48.048027824141499</v>
       </c>
       <c r="H62">
-        <f>AVERAGE(C62:F62)</f>
+        <f t="shared" si="10"/>
         <v>51.284419156397604</v>
       </c>
       <c r="I62">
-        <f>AVERAGE(D62,F62,G62)</f>
+        <f t="shared" si="6"/>
         <v>46.221691483243966</v>
       </c>
       <c r="J62">
-        <f>_xlfn.STDEV.P(D62,F62,G62)</f>
+        <f t="shared" si="7"/>
         <v>2.163137108053844</v>
       </c>
       <c r="K62">
-        <f>_xlfn.STDEV.P(C62:G62)</f>
+        <f t="shared" si="8"/>
         <v>11.930822360420757</v>
       </c>
       <c r="L62" s="4">
-        <f>K62/H62</f>
+        <f t="shared" si="9"/>
         <v>0.2326402942000059</v>
       </c>
       <c r="M62" t="s">
@@ -16989,23 +16991,23 @@
         <v>28.867128747304999</v>
       </c>
       <c r="H63">
-        <f>AVERAGE(C63:F63)</f>
+        <f t="shared" si="10"/>
         <v>50.528482096103652</v>
       </c>
       <c r="I63">
-        <f>AVERAGE(D63,F63,G63)</f>
+        <f t="shared" si="6"/>
         <v>31.206132377239868</v>
       </c>
       <c r="J63">
-        <f>_xlfn.STDEV.P(D63,F63,G63)</f>
+        <f t="shared" si="7"/>
         <v>2.0014086945289185</v>
       </c>
       <c r="K63">
-        <f>_xlfn.STDEV.P(C63:G63)</f>
+        <f t="shared" si="8"/>
         <v>22.777494364805435</v>
       </c>
       <c r="L63" s="4">
-        <f>K63/H63</f>
+        <f t="shared" si="9"/>
         <v>0.45078524863429159</v>
       </c>
       <c r="M63" t="s">
@@ -17050,23 +17052,23 @@
         <v>5.8523965066437</v>
       </c>
       <c r="H64">
-        <f>AVERAGE(C64:F64)</f>
+        <f t="shared" si="10"/>
         <v>25.35554515215151</v>
       </c>
       <c r="I64">
-        <f>AVERAGE(D64,F64,G64)</f>
+        <f t="shared" si="6"/>
         <v>9.2965590384165768</v>
       </c>
       <c r="J64">
-        <f>_xlfn.STDEV.P(D64,F64,G64)</f>
+        <f t="shared" si="7"/>
         <v>3.3632601982570116</v>
       </c>
       <c r="K64">
-        <f>_xlfn.STDEV.P(C64:G64)</f>
+        <f t="shared" si="8"/>
         <v>22.840339621605896</v>
       </c>
       <c r="L64" s="4">
-        <f>K64/H64</f>
+        <f t="shared" si="9"/>
         <v>0.90080254573693552</v>
       </c>
       <c r="M64" t="s">
@@ -17111,23 +17113,23 @@
         <v>4.2202208050945904</v>
       </c>
       <c r="H65">
-        <f>AVERAGE(C65:F65)</f>
+        <f t="shared" si="10"/>
         <v>15.190313766590558</v>
       </c>
       <c r="I65">
-        <f>AVERAGE(D65,F65,G65)</f>
+        <f t="shared" si="6"/>
         <v>6.5881952904856069</v>
       </c>
       <c r="J65">
-        <f>_xlfn.STDEV.P(D65,F65,G65)</f>
+        <f t="shared" si="7"/>
         <v>2.9718081460184522</v>
       </c>
       <c r="K65">
-        <f>_xlfn.STDEV.P(C65:G65)</f>
+        <f t="shared" si="8"/>
         <v>10.297548342483369</v>
       </c>
       <c r="L65" s="4">
-        <f>K65/H65</f>
+        <f t="shared" si="9"/>
         <v>0.67790228040790745</v>
       </c>
       <c r="M65" t="s">
@@ -17172,23 +17174,23 @@
         <v>9.5769138980661008</v>
       </c>
       <c r="H66">
-        <f>AVERAGE(C66:F66)</f>
+        <f t="shared" si="10"/>
         <v>10.976142662728179</v>
       </c>
       <c r="I66">
-        <f>AVERAGE(D66,F66,G66)</f>
+        <f t="shared" ref="I66:I91" si="11">AVERAGE(D66,F66,G66)</f>
         <v>8.2754048496596067</v>
       </c>
       <c r="J66">
-        <f>_xlfn.STDEV.P(D66,F66,G66)</f>
+        <f t="shared" ref="J66:J91" si="12">_xlfn.STDEV.P(D66,F66,G66)</f>
         <v>0.92118768257803618</v>
       </c>
       <c r="K66">
-        <f>_xlfn.STDEV.P(C66:G66)</f>
+        <f t="shared" ref="K66:K97" si="13">_xlfn.STDEV.P(C66:G66)</f>
         <v>3.9040376215215296</v>
       </c>
       <c r="L66" s="4">
-        <f>K66/H66</f>
+        <f t="shared" ref="L66:L97" si="14">K66/H66</f>
         <v>0.35568393573987678</v>
       </c>
       <c r="M66" t="s">
@@ -17233,23 +17235,23 @@
         <v>10.674066278582901</v>
       </c>
       <c r="H67">
-        <f>AVERAGE(C67:F67)</f>
+        <f t="shared" si="10"/>
         <v>7.0181337049043426</v>
       </c>
       <c r="I67">
-        <f>AVERAGE(D67,F67,G67)</f>
+        <f t="shared" si="11"/>
         <v>8.6800766994000895</v>
       </c>
       <c r="J67">
-        <f>_xlfn.STDEV.P(D67,F67,G67)</f>
+        <f t="shared" si="12"/>
         <v>1.5744167379182732</v>
       </c>
       <c r="K67">
-        <f>_xlfn.STDEV.P(C67:G67)</f>
+        <f t="shared" si="13"/>
         <v>3.0670428397212457</v>
       </c>
       <c r="L67" s="4">
-        <f>K67/H67</f>
+        <f t="shared" si="14"/>
         <v>0.43701687210347179</v>
       </c>
       <c r="M67" t="s">
@@ -17294,23 +17296,23 @@
         <v>10.717208322091</v>
       </c>
       <c r="H68">
-        <f>AVERAGE(C68:F68)</f>
+        <f t="shared" si="10"/>
         <v>10.173091076672661</v>
       </c>
       <c r="I68">
-        <f>AVERAGE(D68,F68,G68)</f>
+        <f t="shared" si="11"/>
         <v>9.303072876260547</v>
       </c>
       <c r="J68">
-        <f>_xlfn.STDEV.P(D68,F68,G68)</f>
+        <f t="shared" si="12"/>
         <v>2.4702951754144844</v>
       </c>
       <c r="K68">
-        <f>_xlfn.STDEV.P(C68:G68)</f>
+        <f t="shared" si="13"/>
         <v>6.2636463275334009</v>
       </c>
       <c r="L68" s="4">
-        <f>K68/H68</f>
+        <f t="shared" si="14"/>
         <v>0.61570728899657778</v>
       </c>
       <c r="M68" t="s">
@@ -17355,23 +17357,23 @@
         <v>10.768347908870499</v>
       </c>
       <c r="H69">
-        <f>AVERAGE(C69:F69)</f>
+        <f t="shared" si="10"/>
         <v>8.9791434531660883</v>
       </c>
       <c r="I69">
-        <f>AVERAGE(D69,F69,G69)</f>
+        <f t="shared" si="11"/>
         <v>9.5201349071782868</v>
       </c>
       <c r="J69">
-        <f>_xlfn.STDEV.P(D69,F69,G69)</f>
+        <f t="shared" si="12"/>
         <v>2.0045244821681409</v>
       </c>
       <c r="K69">
-        <f>_xlfn.STDEV.P(C69:G69)</f>
+        <f t="shared" si="13"/>
         <v>2.8783283699557152</v>
       </c>
       <c r="L69" s="4">
-        <f>K69/H69</f>
+        <f t="shared" si="14"/>
         <v>0.32055712050583213</v>
       </c>
       <c r="M69" t="s">
@@ -17416,23 +17418,23 @@
         <v>10.578396745693301</v>
       </c>
       <c r="H70">
-        <f>AVERAGE(C70:F70)</f>
+        <f t="shared" si="10"/>
         <v>10.355335813116776</v>
       </c>
       <c r="I70">
-        <f>AVERAGE(D70,F70,G70)</f>
+        <f t="shared" si="11"/>
         <v>11.500861332720135</v>
       </c>
       <c r="J70">
-        <f>_xlfn.STDEV.P(D70,F70,G70)</f>
+        <f t="shared" si="12"/>
         <v>0.8915872295846532</v>
       </c>
       <c r="K70">
-        <f>_xlfn.STDEV.P(C70:G70)</f>
+        <f t="shared" si="13"/>
         <v>3.6260967546442036</v>
       </c>
       <c r="L70" s="4">
-        <f>K70/H70</f>
+        <f t="shared" si="14"/>
         <v>0.35016698831255105</v>
       </c>
       <c r="M70" t="s">
@@ -17477,23 +17479,23 @@
         <v>8.6562646569683093</v>
       </c>
       <c r="H71">
-        <f>AVERAGE(C71:F71)</f>
+        <f t="shared" si="10"/>
         <v>12.008420222742142</v>
       </c>
       <c r="I71">
-        <f>AVERAGE(D71,F71,G71)</f>
+        <f t="shared" si="11"/>
         <v>9.4351551826456248</v>
       </c>
       <c r="J71">
-        <f>_xlfn.STDEV.P(D71,F71,G71)</f>
+        <f t="shared" si="12"/>
         <v>2.085713865460094</v>
       </c>
       <c r="K71">
-        <f>_xlfn.STDEV.P(C71:G71)</f>
+        <f t="shared" si="13"/>
         <v>3.0467535984822129</v>
       </c>
       <c r="L71" s="4">
-        <f>K71/H71</f>
+        <f t="shared" si="14"/>
         <v>0.25371810296179675</v>
       </c>
       <c r="M71" t="s">
@@ -17538,23 +17540,23 @@
         <v>11.7414573357705</v>
       </c>
       <c r="H72">
-        <f>AVERAGE(C72:F72)</f>
+        <f t="shared" si="10"/>
         <v>12.479476546093544</v>
       </c>
       <c r="I72">
-        <f>AVERAGE(D72,F72,G72)</f>
+        <f t="shared" si="11"/>
         <v>10.06572117338156</v>
       </c>
       <c r="J72">
-        <f>_xlfn.STDEV.P(D72,F72,G72)</f>
+        <f t="shared" si="12"/>
         <v>2.1299997913257167</v>
       </c>
       <c r="K72">
-        <f>_xlfn.STDEV.P(C72:G72)</f>
+        <f t="shared" si="13"/>
         <v>3.2710298952182857</v>
       </c>
       <c r="L72" s="4">
-        <f>K72/H72</f>
+        <f t="shared" si="14"/>
         <v>0.26211274833015474</v>
       </c>
       <c r="M72" t="s">
@@ -17599,23 +17601,23 @@
         <v>15.6735921434102</v>
       </c>
       <c r="H73">
-        <f>AVERAGE(C73:F73)</f>
+        <f t="shared" si="10"/>
         <v>23.262221022590175</v>
       </c>
       <c r="I73">
-        <f>AVERAGE(D73,F73,G73)</f>
+        <f t="shared" si="11"/>
         <v>17.375538744590301</v>
       </c>
       <c r="J73">
-        <f>_xlfn.STDEV.P(D73,F73,G73)</f>
+        <f t="shared" si="12"/>
         <v>1.3276737561286929</v>
       </c>
       <c r="K73">
-        <f>_xlfn.STDEV.P(C73:G73)</f>
+        <f t="shared" si="13"/>
         <v>6.1824480802322741</v>
       </c>
       <c r="L73" s="4">
-        <f>K73/H73</f>
+        <f t="shared" si="14"/>
         <v>0.26577204619577971</v>
       </c>
       <c r="M73" t="s">
@@ -17660,23 +17662,23 @@
         <v>18.764788083403499</v>
       </c>
       <c r="H74">
-        <f>AVERAGE(C74:F74)</f>
+        <f t="shared" ref="H74:H105" si="15">AVERAGE(C74:F74)</f>
         <v>27.749061420821622</v>
       </c>
       <c r="I74">
-        <f>AVERAGE(D74,F74,G74)</f>
+        <f t="shared" si="11"/>
         <v>18.344517922230001</v>
       </c>
       <c r="J74">
-        <f>_xlfn.STDEV.P(D74,F74,G74)</f>
+        <f t="shared" si="12"/>
         <v>0.91075351618826272</v>
       </c>
       <c r="K74">
-        <f>_xlfn.STDEV.P(C74:G74)</f>
+        <f t="shared" si="13"/>
         <v>10.624295312904181</v>
       </c>
       <c r="L74" s="4">
-        <f>K74/H74</f>
+        <f t="shared" si="14"/>
         <v>0.38287043845498131</v>
       </c>
       <c r="M74" t="s">
@@ -17721,23 +17723,23 @@
         <v>11.6115925804387</v>
       </c>
       <c r="H75">
-        <f>AVERAGE(C75:F75)</f>
+        <f t="shared" si="15"/>
         <v>23.379325779672072</v>
       </c>
       <c r="I75">
-        <f>AVERAGE(D75,F75,G75)</f>
+        <f t="shared" si="11"/>
         <v>12.429091899708999</v>
       </c>
       <c r="J75">
-        <f>_xlfn.STDEV.P(D75,F75,G75)</f>
+        <f t="shared" si="12"/>
         <v>0.64442062094195229</v>
       </c>
       <c r="K75">
-        <f>_xlfn.STDEV.P(C75:G75)</f>
+        <f t="shared" si="13"/>
         <v>13.890955353307685</v>
       </c>
       <c r="L75" s="4">
-        <f>K75/H75</f>
+        <f t="shared" si="14"/>
         <v>0.59415551518537102</v>
       </c>
       <c r="M75" t="s">
@@ -17782,23 +17784,23 @@
         <v>11.0212630611852</v>
       </c>
       <c r="H76">
-        <f>AVERAGE(C76:F76)</f>
+        <f t="shared" si="15"/>
         <v>20.796773871051677</v>
       </c>
       <c r="I76">
-        <f>AVERAGE(D76,F76,G76)</f>
+        <f t="shared" si="11"/>
         <v>11.921862848463967</v>
       </c>
       <c r="J76">
-        <f>_xlfn.STDEV.P(D76,F76,G76)</f>
+        <f t="shared" si="12"/>
         <v>0.70090209118052071</v>
       </c>
       <c r="K76">
-        <f>_xlfn.STDEV.P(C76:G76)</f>
+        <f t="shared" si="13"/>
         <v>9.6326044805555746</v>
       </c>
       <c r="L76" s="4">
-        <f>K76/H76</f>
+        <f t="shared" si="14"/>
         <v>0.4631778246126817</v>
       </c>
       <c r="M76" t="s">
@@ -17843,23 +17845,23 @@
         <v>8.6526315646393606</v>
       </c>
       <c r="H77">
-        <f>AVERAGE(C77:F77)</f>
+        <f t="shared" si="15"/>
         <v>18.698862467425826</v>
       </c>
       <c r="I77">
-        <f>AVERAGE(D77,F77,G77)</f>
+        <f t="shared" si="11"/>
         <v>10.149883811447554</v>
       </c>
       <c r="J77">
-        <f>_xlfn.STDEV.P(D77,F77,G77)</f>
+        <f t="shared" si="12"/>
         <v>1.189164194610596</v>
       </c>
       <c r="K77">
-        <f>_xlfn.STDEV.P(C77:G77)</f>
+        <f t="shared" si="13"/>
         <v>8.9889618413835759</v>
       </c>
       <c r="L77" s="4">
-        <f>K77/H77</f>
+        <f t="shared" si="14"/>
         <v>0.48072238923852778</v>
       </c>
       <c r="M77" t="s">
@@ -17904,23 +17906,23 @@
         <v>21.477357509413</v>
       </c>
       <c r="H78">
-        <f>AVERAGE(C78:F78)</f>
+        <f t="shared" si="15"/>
         <v>25.593259994463999</v>
       </c>
       <c r="I78">
-        <f>AVERAGE(D78,F78,G78)</f>
+        <f t="shared" si="11"/>
         <v>24.524605829089666</v>
       </c>
       <c r="J78">
-        <f>_xlfn.STDEV.P(D78,F78,G78)</f>
+        <f t="shared" si="12"/>
         <v>2.1550269508457527</v>
       </c>
       <c r="K78">
-        <f>_xlfn.STDEV.P(C78:G78)</f>
+        <f t="shared" si="13"/>
         <v>8.4998824776648139</v>
       </c>
       <c r="L78" s="4">
-        <f>K78/H78</f>
+        <f t="shared" si="14"/>
         <v>0.33211409877066844</v>
       </c>
       <c r="M78" t="s">
@@ -17965,23 +17967,23 @@
         <v>8.32621758676847</v>
       </c>
       <c r="H79">
-        <f>AVERAGE(C79:F79)</f>
+        <f t="shared" si="15"/>
         <v>16.749921143049576</v>
       </c>
       <c r="I79">
-        <f>AVERAGE(D79,F79,G79)</f>
+        <f t="shared" si="11"/>
         <v>10.307105386322256</v>
       </c>
       <c r="J79">
-        <f>_xlfn.STDEV.P(D79,F79,G79)</f>
+        <f t="shared" si="12"/>
         <v>1.6234942184606937</v>
       </c>
       <c r="K79">
-        <f>_xlfn.STDEV.P(C79:G79)</f>
+        <f t="shared" si="13"/>
         <v>13.614621624938206</v>
       </c>
       <c r="L79" s="4">
-        <f>K79/H79</f>
+        <f t="shared" si="14"/>
         <v>0.81281705798284476</v>
       </c>
       <c r="M79" t="s">
@@ -18026,23 +18028,23 @@
         <v>12.1284998407834</v>
       </c>
       <c r="H80">
-        <f>AVERAGE(C80:F80)</f>
+        <f t="shared" si="15"/>
         <v>13.009635824015676</v>
       </c>
       <c r="I80">
-        <f>AVERAGE(D80,F80,G80)</f>
+        <f t="shared" si="11"/>
         <v>12.120027712282033</v>
       </c>
       <c r="J80">
-        <f>_xlfn.STDEV.P(D80,F80,G80)</f>
+        <f t="shared" si="12"/>
         <v>0.31132337909138452</v>
       </c>
       <c r="K80">
-        <f>_xlfn.STDEV.P(C80:G80)</f>
+        <f t="shared" si="13"/>
         <v>2.6076151597575237</v>
       </c>
       <c r="L80" s="4">
-        <f>K80/H80</f>
+        <f t="shared" si="14"/>
         <v>0.20043721400286152</v>
       </c>
       <c r="M80" t="s">
@@ -18087,23 +18089,23 @@
         <v>11.707384970514401</v>
       </c>
       <c r="H81">
-        <f>AVERAGE(C81:F81)</f>
+        <f t="shared" si="15"/>
         <v>18.473058022999624</v>
       </c>
       <c r="I81">
-        <f>AVERAGE(D81,F81,G81)</f>
+        <f t="shared" si="11"/>
         <v>11.896762354170965</v>
       </c>
       <c r="J81">
-        <f>_xlfn.STDEV.P(D81,F81,G81)</f>
+        <f t="shared" si="12"/>
         <v>0.14815122505809949</v>
       </c>
       <c r="K81">
-        <f>_xlfn.STDEV.P(C81:G81)</f>
+        <f t="shared" si="13"/>
         <v>6.8503978442488647</v>
       </c>
       <c r="L81" s="4">
-        <f>K81/H81</f>
+        <f t="shared" si="14"/>
         <v>0.37083182631266964</v>
       </c>
       <c r="M81" t="s">
@@ -18148,23 +18150,23 @@
         <v>12.017648817912599</v>
       </c>
       <c r="H82">
-        <f>AVERAGE(C82:F82)</f>
+        <f t="shared" si="15"/>
         <v>14.66102344045755</v>
       </c>
       <c r="I82">
-        <f>AVERAGE(D82,F82,G82)</f>
+        <f t="shared" si="11"/>
         <v>12.348511526580934</v>
       </c>
       <c r="J82">
-        <f>_xlfn.STDEV.P(D82,F82,G82)</f>
+        <f t="shared" si="12"/>
         <v>1.2222248696037699</v>
       </c>
       <c r="K82">
-        <f>_xlfn.STDEV.P(C82:G82)</f>
+        <f t="shared" si="13"/>
         <v>10.457123326975134</v>
       </c>
       <c r="L82" s="4">
-        <f>K82/H82</f>
+        <f t="shared" si="14"/>
         <v>0.71326011921639643</v>
       </c>
       <c r="M82" t="s">
@@ -18209,23 +18211,23 @@
         <v>11.8933724868456</v>
       </c>
       <c r="H83">
-        <f>AVERAGE(C83:F83)</f>
+        <f t="shared" si="15"/>
         <v>20.107709117653574</v>
       </c>
       <c r="I83">
-        <f>AVERAGE(D83,F83,G83)</f>
+        <f t="shared" si="11"/>
         <v>13.0869063191533</v>
       </c>
       <c r="J83">
-        <f>_xlfn.STDEV.P(D83,F83,G83)</f>
+        <f t="shared" si="12"/>
         <v>1.4478005520824426</v>
       </c>
       <c r="K83">
-        <f>_xlfn.STDEV.P(C83:G83)</f>
+        <f t="shared" si="13"/>
         <v>7.6105188301596227</v>
       </c>
       <c r="L83" s="4">
-        <f>K83/H83</f>
+        <f t="shared" si="14"/>
         <v>0.3784876131651399</v>
       </c>
       <c r="M83" t="s">
@@ -18270,23 +18272,23 @@
         <v>11.889291732419499</v>
       </c>
       <c r="H84">
-        <f>AVERAGE(C84:F84)</f>
+        <f t="shared" si="15"/>
         <v>19.048514130035656</v>
       </c>
       <c r="I84">
-        <f>AVERAGE(D84,F84,G84)</f>
+        <f t="shared" si="11"/>
         <v>11.435299417520708</v>
       </c>
       <c r="J84">
-        <f>_xlfn.STDEV.P(D84,F84,G84)</f>
+        <f t="shared" si="12"/>
         <v>1.5429517710861576</v>
       </c>
       <c r="K84">
-        <f>_xlfn.STDEV.P(C84:G84)</f>
+        <f t="shared" si="13"/>
         <v>9.3727326715277055</v>
       </c>
       <c r="L84" s="4">
-        <f>K84/H84</f>
+        <f t="shared" si="14"/>
         <v>0.49204534314562631</v>
       </c>
       <c r="M84" t="s">
@@ -18331,23 +18333,23 @@
         <v>24.75041120325</v>
       </c>
       <c r="H85">
-        <f>AVERAGE(C85:F85)</f>
+        <f t="shared" si="15"/>
         <v>34.716757508145299</v>
       </c>
       <c r="I85">
-        <f>AVERAGE(D85,F85,G85)</f>
+        <f t="shared" si="11"/>
         <v>26.512050411943733</v>
       </c>
       <c r="J85">
-        <f>_xlfn.STDEV.P(D85,F85,G85)</f>
+        <f t="shared" si="12"/>
         <v>1.2532571916222075</v>
       </c>
       <c r="K85">
-        <f>_xlfn.STDEV.P(C85:G85)</f>
+        <f t="shared" si="13"/>
         <v>8.0759587311645173</v>
       </c>
       <c r="L85" s="4">
-        <f>K85/H85</f>
+        <f t="shared" si="14"/>
         <v>0.23262422273363875</v>
       </c>
       <c r="M85" t="s">
@@ -18392,23 +18394,23 @@
         <v>20.217338927014001</v>
       </c>
       <c r="H86">
-        <f>AVERAGE(C86:F86)</f>
+        <f t="shared" si="15"/>
         <v>33.907867797630828</v>
       </c>
       <c r="I86">
-        <f>AVERAGE(D86,F86,G86)</f>
+        <f t="shared" si="11"/>
         <v>19.899830039179097</v>
       </c>
       <c r="J86">
-        <f>_xlfn.STDEV.P(D86,F86,G86)</f>
+        <f t="shared" si="12"/>
         <v>0.62640097614439483</v>
       </c>
       <c r="K86">
-        <f>_xlfn.STDEV.P(C86:G86)</f>
+        <f t="shared" si="13"/>
         <v>16.084318090879382</v>
       </c>
       <c r="L86" s="4">
-        <f>K86/H86</f>
+        <f t="shared" si="14"/>
         <v>0.47435356852497834</v>
       </c>
       <c r="M86" t="s">
@@ -18453,23 +18455,23 @@
         <v>27.2903666766863</v>
       </c>
       <c r="H87">
-        <f>AVERAGE(C87:F87)</f>
+        <f t="shared" si="15"/>
         <v>36.763967828824079</v>
       </c>
       <c r="I87">
-        <f>AVERAGE(D87,F87,G87)</f>
+        <f t="shared" si="11"/>
         <v>25.6602426639942</v>
       </c>
       <c r="J87">
-        <f>_xlfn.STDEV.P(D87,F87,G87)</f>
+        <f t="shared" si="12"/>
         <v>1.4912014373289546</v>
       </c>
       <c r="K87">
-        <f>_xlfn.STDEV.P(C87:G87)</f>
+        <f t="shared" si="13"/>
         <v>12.270504409315642</v>
       </c>
       <c r="L87" s="4">
-        <f>K87/H87</f>
+        <f t="shared" si="14"/>
         <v>0.33376442027280823</v>
       </c>
       <c r="M87" t="s">
@@ -18514,23 +18516,23 @@
         <v>17.7696158758996</v>
       </c>
       <c r="H88">
-        <f>AVERAGE(C88:F88)</f>
+        <f t="shared" si="15"/>
         <v>29.408046203867102</v>
       </c>
       <c r="I88">
-        <f>AVERAGE(D88,F88,G88)</f>
+        <f t="shared" si="11"/>
         <v>16.944683563789336</v>
       </c>
       <c r="J88">
-        <f>_xlfn.STDEV.P(D88,F88,G88)</f>
+        <f t="shared" si="12"/>
         <v>0.77890077499248533</v>
       </c>
       <c r="K88">
-        <f>_xlfn.STDEV.P(C88:G88)</f>
+        <f t="shared" si="13"/>
         <v>17.196208419959436</v>
       </c>
       <c r="L88" s="4">
-        <f>K88/H88</f>
+        <f t="shared" si="14"/>
         <v>0.58474501504619403</v>
       </c>
       <c r="M88" t="s">
@@ -18575,23 +18577,23 @@
         <v>18.442798818957701</v>
       </c>
       <c r="H89">
-        <f>AVERAGE(C89:F89)</f>
+        <f t="shared" si="15"/>
         <v>27.879578763241927</v>
       </c>
       <c r="I89">
-        <f>AVERAGE(D89,F89,G89)</f>
+        <f t="shared" si="11"/>
         <v>18.5836612906418</v>
       </c>
       <c r="J89">
-        <f>_xlfn.STDEV.P(D89,F89,G89)</f>
+        <f t="shared" si="12"/>
         <v>0.15768991538325353</v>
       </c>
       <c r="K89">
-        <f>_xlfn.STDEV.P(C89:G89)</f>
+        <f t="shared" si="13"/>
         <v>9.8507646763844949</v>
       </c>
       <c r="L89" s="4">
-        <f>K89/H89</f>
+        <f t="shared" si="14"/>
         <v>0.35333262242011781</v>
       </c>
       <c r="M89" t="s">
@@ -18636,23 +18638,23 @@
         <v>17.417029045003201</v>
       </c>
       <c r="H90">
-        <f>AVERAGE(C90:F90)</f>
+        <f t="shared" si="15"/>
         <v>27.527479303856225</v>
       </c>
       <c r="I90">
-        <f>AVERAGE(D90,F90,G90)</f>
+        <f t="shared" si="11"/>
         <v>16.678308753476035</v>
       </c>
       <c r="J90">
-        <f>_xlfn.STDEV.P(D90,F90,G90)</f>
+        <f t="shared" si="12"/>
         <v>0.82524524675733635</v>
       </c>
       <c r="K90">
-        <f>_xlfn.STDEV.P(C90:G90)</f>
+        <f t="shared" si="13"/>
         <v>13.557542430411864</v>
       </c>
       <c r="L90" s="4">
-        <f>K90/H90</f>
+        <f t="shared" si="14"/>
         <v>0.49250940417608952</v>
       </c>
       <c r="M90" t="s">
@@ -18697,23 +18699,23 @@
         <v>18.538759036861698</v>
       </c>
       <c r="H91">
-        <f>AVERAGE(C91:F91)</f>
+        <f t="shared" si="15"/>
         <v>23.266345375050353</v>
       </c>
       <c r="I91">
-        <f>AVERAGE(D91,F91,G91)</f>
+        <f t="shared" si="11"/>
         <v>16.309363512354366</v>
       </c>
       <c r="J91">
-        <f>_xlfn.STDEV.P(D91,F91,G91)</f>
+        <f t="shared" si="12"/>
         <v>1.7377689706383124</v>
       </c>
       <c r="K91">
-        <f>_xlfn.STDEV.P(C91:G91)</f>
+        <f t="shared" si="13"/>
         <v>8.6634407919334464</v>
       </c>
       <c r="L91" s="4">
-        <f>K91/H91</f>
+        <f t="shared" si="14"/>
         <v>0.37235933071051547</v>
       </c>
       <c r="M91" t="s">
@@ -18754,15 +18756,15 @@
       <c r="F92" s="12"/>
       <c r="G92" s="12"/>
       <c r="H92">
-        <f>AVERAGE(C92:F92)</f>
+        <f t="shared" si="15"/>
         <v>30.440010549529234</v>
       </c>
       <c r="K92">
-        <f>_xlfn.STDEV.P(C92:G92)</f>
+        <f t="shared" si="13"/>
         <v>0.27913131935003588</v>
       </c>
       <c r="L92">
-        <f>K92/H92</f>
+        <f t="shared" si="14"/>
         <v>9.1698824774012026E-3</v>
       </c>
       <c r="M92" t="s">
@@ -18794,15 +18796,15 @@
       <c r="F93" s="12"/>
       <c r="G93" s="12"/>
       <c r="H93">
-        <f>AVERAGE(C93:F93)</f>
+        <f t="shared" si="15"/>
         <v>181.85500125976304</v>
       </c>
       <c r="K93">
-        <f>_xlfn.STDEV.P(C93:G93)</f>
+        <f t="shared" si="13"/>
         <v>20.134181733470101</v>
       </c>
       <c r="L93">
-        <f>K93/H93</f>
+        <f t="shared" si="14"/>
         <v>0.11071557886225128</v>
       </c>
       <c r="M93" t="s">
@@ -18834,15 +18836,15 @@
       <c r="F94" s="12"/>
       <c r="G94" s="12"/>
       <c r="H94">
-        <f>AVERAGE(C94:F94)</f>
+        <f t="shared" si="15"/>
         <v>21.593535325214834</v>
       </c>
       <c r="K94">
-        <f>_xlfn.STDEV.P(C94:G94)</f>
+        <f t="shared" si="13"/>
         <v>1.757558707146031</v>
       </c>
       <c r="L94">
-        <f>K94/H94</f>
+        <f t="shared" si="14"/>
         <v>8.1392818761535757E-2</v>
       </c>
       <c r="M94" t="s">
@@ -18874,15 +18876,15 @@
       <c r="F95" s="12"/>
       <c r="G95" s="12"/>
       <c r="H95">
-        <f>AVERAGE(C95:F95)</f>
+        <f t="shared" si="15"/>
         <v>20.247576669166335</v>
       </c>
       <c r="K95">
-        <f>_xlfn.STDEV.P(C95:G95)</f>
+        <f t="shared" si="13"/>
         <v>0.68605746128762457</v>
       </c>
       <c r="L95">
-        <f>K95/H95</f>
+        <f t="shared" si="14"/>
         <v>3.3883435657382895E-2</v>
       </c>
       <c r="M95" t="s">
@@ -18914,15 +18916,15 @@
       <c r="F96" s="12"/>
       <c r="G96" s="12"/>
       <c r="H96">
-        <f>AVERAGE(C96:F96)</f>
+        <f t="shared" si="15"/>
         <v>187.06655931293631</v>
       </c>
       <c r="K96">
-        <f>_xlfn.STDEV.P(C96:G96)</f>
+        <f t="shared" si="13"/>
         <v>27.287487419434701</v>
       </c>
       <c r="L96">
-        <f>K96/H96</f>
+        <f t="shared" si="14"/>
         <v>0.14587047262566333</v>
       </c>
       <c r="M96" t="s">
@@ -18954,15 +18956,15 @@
       <c r="F97" s="12"/>
       <c r="G97" s="12"/>
       <c r="H97">
-        <f>AVERAGE(C97:F97)</f>
+        <f t="shared" si="15"/>
         <v>19.396004296683834</v>
       </c>
       <c r="K97">
-        <f>_xlfn.STDEV.P(C97:G97)</f>
+        <f t="shared" si="13"/>
         <v>1.3983112671597304</v>
       </c>
       <c r="L97">
-        <f>K97/H97</f>
+        <f t="shared" si="14"/>
         <v>7.209274888636738E-2</v>
       </c>
       <c r="M97" t="s">
@@ -18992,15 +18994,15 @@
         <v>14.817036887393099</v>
       </c>
       <c r="H98">
-        <f>AVERAGE(C98:F98)</f>
+        <f t="shared" si="15"/>
         <v>17.495456951090233</v>
       </c>
       <c r="K98">
-        <f>_xlfn.STDEV.P(C98:G98)</f>
+        <f t="shared" ref="K98:K129" si="16">_xlfn.STDEV.P(C98:G98)</f>
         <v>1.9060477565132941</v>
       </c>
       <c r="L98">
-        <f>K98/H98</f>
+        <f t="shared" ref="L98:L129" si="17">K98/H98</f>
         <v>0.10894529716153074</v>
       </c>
       <c r="M98" t="s">
@@ -19032,15 +19034,15 @@
       <c r="F99" s="10"/>
       <c r="G99" s="10"/>
       <c r="H99">
-        <f>AVERAGE(C99:F99)</f>
+        <f t="shared" si="15"/>
         <v>178.55542136339236</v>
       </c>
       <c r="K99">
-        <f>_xlfn.STDEV.P(C99:G99)</f>
+        <f t="shared" si="16"/>
         <v>17.614541914451781</v>
       </c>
       <c r="L99">
-        <f>K99/H99</f>
+        <f t="shared" si="17"/>
         <v>9.8650277767836705E-2</v>
       </c>
       <c r="M99" t="s">
@@ -19072,15 +19074,15 @@
       <c r="F100" s="10"/>
       <c r="G100" s="10"/>
       <c r="H100">
-        <f>AVERAGE(C100:F100)</f>
+        <f t="shared" si="15"/>
         <v>16.821059067926232</v>
       </c>
       <c r="K100">
-        <f>_xlfn.STDEV.P(C100:G100)</f>
+        <f t="shared" si="16"/>
         <v>2.1921723850996457</v>
       </c>
       <c r="L100">
-        <f>K100/H100</f>
+        <f t="shared" si="17"/>
         <v>0.13032308942304341</v>
       </c>
       <c r="M100" t="s">
@@ -19112,15 +19114,15 @@
       <c r="F101" s="10"/>
       <c r="G101" s="10"/>
       <c r="H101">
-        <f>AVERAGE(C101:F101)</f>
+        <f t="shared" si="15"/>
         <v>15.798994909233967</v>
       </c>
       <c r="K101">
-        <f>_xlfn.STDEV.P(C101:G101)</f>
+        <f t="shared" si="16"/>
         <v>1.1682355946463394</v>
       </c>
       <c r="L101">
-        <f>K101/H101</f>
+        <f t="shared" si="17"/>
         <v>7.3943665489982921E-2</v>
       </c>
       <c r="M101" t="s">
@@ -19152,15 +19154,15 @@
       <c r="F102" s="10"/>
       <c r="G102" s="10"/>
       <c r="H102">
-        <f>AVERAGE(C102:F102)</f>
+        <f t="shared" si="15"/>
         <v>16.063767641496867</v>
       </c>
       <c r="K102">
-        <f>_xlfn.STDEV.P(C102:G102)</f>
+        <f t="shared" si="16"/>
         <v>1.7296212445288115</v>
       </c>
       <c r="L102">
-        <f>K102/H102</f>
+        <f t="shared" si="17"/>
         <v>0.10767220263201221</v>
       </c>
       <c r="M102" t="s">
@@ -19192,15 +19194,15 @@
       <c r="F103" s="10"/>
       <c r="G103" s="10"/>
       <c r="H103">
-        <f>AVERAGE(C103:F103)</f>
+        <f t="shared" si="15"/>
         <v>19.682277378864132</v>
       </c>
       <c r="K103">
-        <f>_xlfn.STDEV.P(C103:G103)</f>
+        <f t="shared" si="16"/>
         <v>2.4105744692201534</v>
       </c>
       <c r="L103">
-        <f>K103/H103</f>
+        <f t="shared" si="17"/>
         <v>0.12247436731121143</v>
       </c>
       <c r="M103" t="s">
@@ -19232,15 +19234,15 @@
       <c r="F104" s="10"/>
       <c r="G104" s="10"/>
       <c r="H104">
-        <f>AVERAGE(C104:F104)</f>
+        <f t="shared" si="15"/>
         <v>205.66022544283399</v>
       </c>
       <c r="K104">
-        <f>_xlfn.STDEV.P(C104:G104)</f>
+        <f t="shared" si="16"/>
         <v>23.613882537152339</v>
       </c>
       <c r="L104">
-        <f>K104/H104</f>
+        <f t="shared" si="17"/>
         <v>0.11481988063713434</v>
       </c>
       <c r="M104" t="s">
@@ -19272,15 +19274,15 @@
       <c r="F105" s="10"/>
       <c r="G105" s="10"/>
       <c r="H105">
-        <f>AVERAGE(C105:F105)</f>
+        <f t="shared" si="15"/>
         <v>19.521604992889497</v>
       </c>
       <c r="K105">
-        <f>_xlfn.STDEV.P(C105:G105)</f>
+        <f t="shared" si="16"/>
         <v>1.3732810408426013</v>
       </c>
       <c r="L105">
-        <f>K105/H105</f>
+        <f t="shared" si="17"/>
         <v>7.0346728219467705E-2</v>
       </c>
       <c r="M105" t="s">
@@ -19312,15 +19314,15 @@
       <c r="F106" s="10"/>
       <c r="G106" s="10"/>
       <c r="H106">
-        <f>AVERAGE(C106:F106)</f>
+        <f t="shared" ref="H106:H137" si="18">AVERAGE(C106:F106)</f>
         <v>15.8130927284812</v>
       </c>
       <c r="K106">
-        <f>_xlfn.STDEV.P(C106:G106)</f>
+        <f t="shared" si="16"/>
         <v>1.4716378797533274</v>
       </c>
       <c r="L106">
-        <f>K106/H106</f>
+        <f t="shared" si="17"/>
         <v>9.3064519700358062E-2</v>
       </c>
       <c r="M106" t="s">
@@ -19352,15 +19354,15 @@
       <c r="F107" s="10"/>
       <c r="G107" s="10"/>
       <c r="H107">
-        <f>AVERAGE(C107:F107)</f>
+        <f t="shared" si="18"/>
         <v>12.002522758824705</v>
       </c>
       <c r="K107">
-        <f>_xlfn.STDEV.P(C107:G107)</f>
+        <f t="shared" si="16"/>
         <v>2.5101162868813893</v>
       </c>
       <c r="L107">
-        <f>K107/H107</f>
+        <f t="shared" si="17"/>
         <v>0.20913239135796327</v>
       </c>
       <c r="M107" t="s">
@@ -19392,15 +19394,15 @@
       <c r="F108" s="10"/>
       <c r="G108" s="10"/>
       <c r="H108">
-        <f>AVERAGE(C108:F108)</f>
+        <f t="shared" si="18"/>
         <v>10.267414901272227</v>
       </c>
       <c r="K108">
-        <f>_xlfn.STDEV.P(C108:G108)</f>
+        <f t="shared" si="16"/>
         <v>3.1773075322803783</v>
       </c>
       <c r="L108">
-        <f>K108/H108</f>
+        <f t="shared" si="17"/>
         <v>0.30945545327935281</v>
       </c>
       <c r="M108" t="s">
@@ -19432,15 +19434,15 @@
       <c r="F109" s="10"/>
       <c r="G109" s="10"/>
       <c r="H109">
-        <f>AVERAGE(C109:F109)</f>
+        <f t="shared" si="18"/>
         <v>10.306472135750285</v>
       </c>
       <c r="K109">
-        <f>_xlfn.STDEV.P(C109:G109)</f>
+        <f t="shared" si="16"/>
         <v>2.2311122397195744</v>
       </c>
       <c r="L109">
-        <f>K109/H109</f>
+        <f t="shared" si="17"/>
         <v>0.21647681285436815</v>
       </c>
       <c r="M109" t="s">
@@ -19472,15 +19474,15 @@
       <c r="F110" s="10"/>
       <c r="G110" s="10"/>
       <c r="H110">
-        <f>AVERAGE(C110:F110)</f>
+        <f t="shared" si="18"/>
         <v>10.380402578636962</v>
       </c>
       <c r="K110">
-        <f>_xlfn.STDEV.P(C110:G110)</f>
+        <f t="shared" si="16"/>
         <v>2.8657503439162966</v>
       </c>
       <c r="L110">
-        <f>K110/H110</f>
+        <f t="shared" si="17"/>
         <v>0.27607314092172663</v>
       </c>
       <c r="M110" t="s">
@@ -19512,15 +19514,15 @@
       <c r="F111" s="10"/>
       <c r="G111" s="10"/>
       <c r="H111">
-        <f>AVERAGE(C111:F111)</f>
+        <f t="shared" si="18"/>
         <v>8.1390659077696199</v>
       </c>
       <c r="K111">
-        <f>_xlfn.STDEV.P(C111:G111)</f>
+        <f t="shared" si="16"/>
         <v>1.2802855120710934</v>
       </c>
       <c r="L111">
-        <f>K111/H111</f>
+        <f t="shared" si="17"/>
         <v>0.15730128328963675</v>
       </c>
       <c r="M111" t="s">
@@ -19552,15 +19554,15 @@
       <c r="F112" s="10"/>
       <c r="G112" s="10"/>
       <c r="H112">
-        <f>AVERAGE(C112:F112)</f>
+        <f t="shared" si="18"/>
         <v>8.668695786141372</v>
       </c>
       <c r="K112">
-        <f>_xlfn.STDEV.P(C112:G112)</f>
+        <f t="shared" si="16"/>
         <v>2.5073326532306717</v>
       </c>
       <c r="L112">
-        <f>K112/H112</f>
+        <f t="shared" si="17"/>
         <v>0.28923989433787028</v>
       </c>
       <c r="M112" t="s">
@@ -19592,15 +19594,15 @@
       <c r="F113" s="10"/>
       <c r="G113" s="10"/>
       <c r="H113">
-        <f>AVERAGE(C113:F113)</f>
+        <f t="shared" si="18"/>
         <v>149.68843149347302</v>
       </c>
       <c r="K113">
-        <f>_xlfn.STDEV.P(C113:G113)</f>
+        <f t="shared" si="16"/>
         <v>20.07534215226125</v>
       </c>
       <c r="L113">
-        <f>K113/H113</f>
+        <f t="shared" si="17"/>
         <v>0.13411418605943914</v>
       </c>
       <c r="M113" t="s">
@@ -19632,15 +19634,15 @@
       <c r="F114" s="10"/>
       <c r="G114" s="10"/>
       <c r="H114">
-        <f>AVERAGE(C114:F114)</f>
+        <f t="shared" si="18"/>
         <v>157.59057971014468</v>
       </c>
       <c r="K114">
-        <f>_xlfn.STDEV.P(C114:G114)</f>
+        <f t="shared" si="16"/>
         <v>16.752084986554976</v>
       </c>
       <c r="L114">
-        <f>K114/H114</f>
+        <f t="shared" si="17"/>
         <v>0.10630130949049732</v>
       </c>
       <c r="M114" t="s">
@@ -19672,15 +19674,15 @@
       <c r="F115" s="10"/>
       <c r="G115" s="10"/>
       <c r="H115">
-        <f>AVERAGE(C115:F115)</f>
+        <f t="shared" si="18"/>
         <v>34.039485205565462</v>
       </c>
       <c r="K115">
-        <f>_xlfn.STDEV.P(C115:G115)</f>
+        <f t="shared" si="16"/>
         <v>1.073155830754688</v>
       </c>
       <c r="L115">
-        <f>K115/H115</f>
+        <f t="shared" si="17"/>
         <v>3.1526793788856325E-2</v>
       </c>
       <c r="M115" t="s">
@@ -19712,15 +19714,15 @@
       <c r="F116" s="10"/>
       <c r="G116" s="10"/>
       <c r="H116">
-        <f>AVERAGE(C116:F116)</f>
+        <f t="shared" si="18"/>
         <v>200.87886717415699</v>
       </c>
       <c r="K116">
-        <f>_xlfn.STDEV.P(C116:G116)</f>
+        <f t="shared" si="16"/>
         <v>22.124666439360507</v>
       </c>
       <c r="L116">
-        <f>K116/H116</f>
+        <f t="shared" si="17"/>
         <v>0.11013934293137451</v>
       </c>
       <c r="M116" t="s">
@@ -19752,15 +19754,15 @@
       <c r="F117" s="10"/>
       <c r="G117" s="10"/>
       <c r="H117">
-        <f>AVERAGE(C117:F117)</f>
+        <f t="shared" si="18"/>
         <v>169.56790123456767</v>
       </c>
       <c r="K117">
-        <f>_xlfn.STDEV.P(C117:G117)</f>
+        <f t="shared" si="16"/>
         <v>15.242539483531898</v>
       </c>
       <c r="L117">
-        <f>K117/H117</f>
+        <f t="shared" si="17"/>
         <v>8.9890476750352055E-2</v>
       </c>
       <c r="M117" t="s">
@@ -19792,15 +19794,15 @@
       <c r="F118" s="10"/>
       <c r="G118" s="10"/>
       <c r="H118">
-        <f>AVERAGE(C118:F118)</f>
+        <f t="shared" si="18"/>
         <v>164.42498658078367</v>
       </c>
       <c r="K118">
-        <f>_xlfn.STDEV.P(C118:G118)</f>
+        <f t="shared" si="16"/>
         <v>19.177250320565008</v>
       </c>
       <c r="L118">
-        <f>K118/H118</f>
+        <f t="shared" si="17"/>
         <v>0.11663221460044353</v>
       </c>
       <c r="M118" t="s">
@@ -19832,15 +19834,15 @@
       <c r="F119" s="10"/>
       <c r="G119" s="10"/>
       <c r="H119">
-        <f>AVERAGE(C119:F119)</f>
+        <f t="shared" si="18"/>
         <v>163.33333333333334</v>
       </c>
       <c r="K119">
-        <f>_xlfn.STDEV.P(C119:G119)</f>
+        <f t="shared" si="16"/>
         <v>21.137221237139912</v>
       </c>
       <c r="L119">
-        <f>K119/H119</f>
+        <f t="shared" si="17"/>
         <v>0.12941155859473413</v>
       </c>
       <c r="M119" t="s">
@@ -19872,15 +19874,15 @@
       <c r="F120" s="10"/>
       <c r="G120" s="10"/>
       <c r="H120">
-        <f>AVERAGE(C120:F120)</f>
+        <f t="shared" si="18"/>
         <v>151.56169698838502</v>
       </c>
       <c r="K120">
-        <f>_xlfn.STDEV.P(C120:G120)</f>
+        <f t="shared" si="16"/>
         <v>16.608652315828699</v>
       </c>
       <c r="L120">
-        <f>K120/H120</f>
+        <f t="shared" si="17"/>
         <v>0.10958344123780502</v>
       </c>
       <c r="M120" t="s">
@@ -19912,15 +19914,15 @@
       <c r="F121" s="10"/>
       <c r="G121" s="10"/>
       <c r="H121">
-        <f>AVERAGE(C121:F121)</f>
+        <f t="shared" si="18"/>
         <v>14.875922908362233</v>
       </c>
       <c r="K121">
-        <f>_xlfn.STDEV.P(C121:G121)</f>
+        <f t="shared" si="16"/>
         <v>0.51974707917229923</v>
       </c>
       <c r="L121">
-        <f>K121/H121</f>
+        <f t="shared" si="17"/>
         <v>3.4938812359677718E-2</v>
       </c>
       <c r="M121" t="s">
@@ -19952,15 +19954,15 @@
       <c r="F122" s="10"/>
       <c r="G122" s="10"/>
       <c r="H122">
-        <f>AVERAGE(C122:F122)</f>
+        <f t="shared" si="18"/>
         <v>149.31226516371433</v>
       </c>
       <c r="K122">
-        <f>_xlfn.STDEV.P(C122:G122)</f>
+        <f t="shared" si="16"/>
         <v>20.281515894040112</v>
       </c>
       <c r="L122">
-        <f>K122/H122</f>
+        <f t="shared" si="17"/>
         <v>0.13583288601108773</v>
       </c>
       <c r="M122" t="s">
@@ -19992,15 +19994,15 @@
       <c r="F123" s="10"/>
       <c r="G123" s="10"/>
       <c r="H123">
-        <f>AVERAGE(C123:F123)</f>
+        <f t="shared" si="18"/>
         <v>140.97423510466999</v>
       </c>
       <c r="K123">
-        <f>_xlfn.STDEV.P(C123:G123)</f>
+        <f t="shared" si="16"/>
         <v>20.43988634937406</v>
       </c>
       <c r="L123">
-        <f>K123/H123</f>
+        <f t="shared" si="17"/>
         <v>0.14499022700281322</v>
       </c>
       <c r="M123" t="s">
@@ -20032,15 +20034,15 @@
       <c r="F124" s="10"/>
       <c r="G124" s="10"/>
       <c r="H124">
-        <f>AVERAGE(C124:F124)</f>
+        <f t="shared" si="18"/>
         <v>143.14009661835735</v>
       </c>
       <c r="K124">
-        <f>_xlfn.STDEV.P(C124:G124)</f>
+        <f t="shared" si="16"/>
         <v>27.303496718258462</v>
       </c>
       <c r="L124">
-        <f>K124/H124</f>
+        <f t="shared" si="17"/>
         <v>0.19074666961456319</v>
       </c>
       <c r="M124" t="s">
@@ -20072,15 +20074,15 @@
       <c r="F125" s="10"/>
       <c r="G125" s="10"/>
       <c r="H125">
-        <f>AVERAGE(C125:F125)</f>
+        <f t="shared" si="18"/>
         <v>138.28695138246468</v>
       </c>
       <c r="K125">
-        <f>_xlfn.STDEV.P(C125:G125)</f>
+        <f t="shared" si="16"/>
         <v>23.323496493846122</v>
       </c>
       <c r="L125">
-        <f>K125/H125</f>
+        <f t="shared" si="17"/>
         <v>0.16866013937453561</v>
       </c>
       <c r="M125" t="s">
@@ -20112,15 +20114,15 @@
       <c r="F126" s="10"/>
       <c r="G126" s="10"/>
       <c r="H126">
-        <f>AVERAGE(C126:F126)</f>
+        <f t="shared" si="18"/>
         <v>142.52960443436666</v>
       </c>
       <c r="K126">
-        <f>_xlfn.STDEV.P(C126:G126)</f>
+        <f t="shared" si="16"/>
         <v>20.814858896100482</v>
       </c>
       <c r="L126">
-        <f>K126/H126</f>
+        <f t="shared" si="17"/>
         <v>0.14603884560477748</v>
       </c>
       <c r="M126" t="s">
@@ -20152,15 +20154,15 @@
       <c r="F127" s="10"/>
       <c r="G127" s="10"/>
       <c r="H127">
-        <f>AVERAGE(C127:F127)</f>
+        <f t="shared" si="18"/>
         <v>168.44873859366601</v>
       </c>
       <c r="K127">
-        <f>_xlfn.STDEV.P(C127:G127)</f>
+        <f t="shared" si="16"/>
         <v>18.268944850179224</v>
       </c>
       <c r="L127">
-        <f>K127/H127</f>
+        <f t="shared" si="17"/>
         <v>0.10845403178855369</v>
       </c>
       <c r="M127" t="s">
@@ -20192,15 +20194,15 @@
       <c r="F128" s="10"/>
       <c r="G128" s="10"/>
       <c r="H128">
-        <f>AVERAGE(C128:F128)</f>
+        <f t="shared" si="18"/>
         <v>222.74020397208801</v>
       </c>
       <c r="K128">
-        <f>_xlfn.STDEV.P(C128:G128)</f>
+        <f t="shared" si="16"/>
         <v>21.670881910998638</v>
       </c>
       <c r="L128">
-        <f>K128/H128</f>
+        <f t="shared" si="17"/>
         <v>9.729218849828411E-2</v>
       </c>
       <c r="M128" t="s">
@@ -20232,15 +20234,15 @@
       <c r="F129" s="10"/>
       <c r="G129" s="10"/>
       <c r="H129">
-        <f>AVERAGE(C129:F129)</f>
+        <f t="shared" si="18"/>
         <v>177.99986580783698</v>
       </c>
       <c r="K129">
-        <f>_xlfn.STDEV.P(C129:G129)</f>
+        <f t="shared" si="16"/>
         <v>22.345721420800277</v>
       </c>
       <c r="L129">
-        <f>K129/H129</f>
+        <f t="shared" si="17"/>
         <v>0.12553785543256538</v>
       </c>
       <c r="M129" t="s">
@@ -20272,15 +20274,15 @@
       <c r="F130" s="10"/>
       <c r="G130" s="10"/>
       <c r="H130">
-        <f>AVERAGE(C130:F130)</f>
+        <f t="shared" si="18"/>
         <v>166.08024691358</v>
       </c>
       <c r="K130">
-        <f>_xlfn.STDEV.P(C130:G130)</f>
+        <f t="shared" ref="K130:K161" si="19">_xlfn.STDEV.P(C130:G130)</f>
         <v>17.729218231172808</v>
       </c>
       <c r="L130">
-        <f>K130/H130</f>
+        <f t="shared" ref="L130:L161" si="20">K130/H130</f>
         <v>0.10675091445642071</v>
       </c>
       <c r="M130" t="s">
@@ -20312,15 +20314,15 @@
       <c r="F131" s="10"/>
       <c r="G131" s="10"/>
       <c r="H131">
-        <f>AVERAGE(C131:F131)</f>
+        <f t="shared" si="18"/>
         <v>17.9353752457213</v>
       </c>
       <c r="K131">
-        <f>_xlfn.STDEV.P(C131:G131)</f>
+        <f t="shared" si="19"/>
         <v>0.70178954691852624</v>
       </c>
       <c r="L131">
-        <f>K131/H131</f>
+        <f t="shared" si="20"/>
         <v>3.9128790856268622E-2</v>
       </c>
       <c r="M131" t="s">
@@ -20352,15 +20354,15 @@
       <c r="F132" s="10"/>
       <c r="G132" s="10"/>
       <c r="H132">
-        <f>AVERAGE(C132:F132)</f>
+        <f t="shared" si="18"/>
         <v>151.01851851851868</v>
       </c>
       <c r="K132">
-        <f>_xlfn.STDEV.P(C132:G132)</f>
+        <f t="shared" si="19"/>
         <v>16.674038150357973</v>
       </c>
       <c r="L132">
-        <f>K132/H132</f>
+        <f t="shared" si="20"/>
         <v>0.11041055304958057</v>
       </c>
       <c r="M132" t="s">
@@ -20392,15 +20394,15 @@
       <c r="F133" s="10"/>
       <c r="G133" s="10"/>
       <c r="H133">
-        <f>AVERAGE(C133:F133)</f>
+        <f t="shared" si="18"/>
         <v>154.28542673107899</v>
       </c>
       <c r="K133">
-        <f>_xlfn.STDEV.P(C133:G133)</f>
+        <f t="shared" si="19"/>
         <v>14.580499139853934</v>
       </c>
       <c r="L133">
-        <f>K133/H133</f>
+        <f t="shared" si="20"/>
         <v>9.4503411299291976E-2</v>
       </c>
       <c r="M133" t="s">
@@ -20432,15 +20434,15 @@
       <c r="F134" s="10"/>
       <c r="G134" s="10"/>
       <c r="H134">
-        <f>AVERAGE(C134:F134)</f>
+        <f t="shared" si="18"/>
         <v>12.098520072763696</v>
       </c>
       <c r="K134">
-        <f>_xlfn.STDEV.P(C134:G134)</f>
+        <f t="shared" si="19"/>
         <v>2.4748776057144819</v>
       </c>
       <c r="L134">
-        <f>K134/H134</f>
+        <f t="shared" si="20"/>
         <v>0.20456035869097328</v>
       </c>
       <c r="M134" t="s">
@@ -20472,15 +20474,15 @@
       <c r="F135" s="10"/>
       <c r="G135" s="10"/>
       <c r="H135">
-        <f>AVERAGE(C135:F135)</f>
+        <f t="shared" si="18"/>
         <v>24.926472974699298</v>
       </c>
       <c r="K135">
-        <f>_xlfn.STDEV.P(C135:G135)</f>
+        <f t="shared" si="19"/>
         <v>0.5967925872320744</v>
       </c>
       <c r="L135">
-        <f>K135/H135</f>
+        <f t="shared" si="20"/>
         <v>2.3942119201454087E-2</v>
       </c>
       <c r="M135" t="s">
@@ -20512,15 +20514,15 @@
       <c r="F136" s="10"/>
       <c r="G136" s="10"/>
       <c r="H136">
-        <f>AVERAGE(C136:F136)</f>
+        <f t="shared" si="18"/>
         <v>11.763832113587801</v>
       </c>
       <c r="K136">
-        <f>_xlfn.STDEV.P(C136:G136)</f>
+        <f t="shared" si="19"/>
         <v>1.0297397879475056</v>
       </c>
       <c r="L136">
-        <f>K136/H136</f>
+        <f t="shared" si="20"/>
         <v>8.7534383184379672E-2</v>
       </c>
       <c r="M136" t="s">
@@ -20552,15 +20554,15 @@
       <c r="F137" s="10"/>
       <c r="G137" s="10"/>
       <c r="H137">
-        <f>AVERAGE(C137:F137)</f>
+        <f t="shared" si="18"/>
         <v>6.2364563386574545</v>
       </c>
       <c r="K137">
-        <f>_xlfn.STDEV.P(C137:G137)</f>
+        <f t="shared" si="19"/>
         <v>3.8584286466797879</v>
       </c>
       <c r="L137">
-        <f>K137/H137</f>
+        <f t="shared" si="20"/>
         <v>0.61868927435005605</v>
       </c>
       <c r="M137" t="s">
@@ -20592,15 +20594,15 @@
       <c r="F138" s="10"/>
       <c r="G138" s="10"/>
       <c r="H138">
-        <f>AVERAGE(C138:F138)</f>
+        <f t="shared" ref="H138:H169" si="21">AVERAGE(C138:F138)</f>
         <v>5.5239679140411937</v>
       </c>
       <c r="K138">
-        <f>_xlfn.STDEV.P(C138:G138)</f>
+        <f t="shared" si="19"/>
         <v>3.2756729322826676</v>
       </c>
       <c r="L138">
-        <f>K138/H138</f>
+        <f t="shared" si="20"/>
         <v>0.59299275145250963</v>
       </c>
       <c r="M138" t="s">
@@ -20632,15 +20634,15 @@
       <c r="F139" s="10"/>
       <c r="G139" s="10"/>
       <c r="H139">
-        <f>AVERAGE(C139:F139)</f>
+        <f t="shared" si="21"/>
         <v>42.406487850311862</v>
       </c>
       <c r="K139">
-        <f>_xlfn.STDEV.P(C139:G139)</f>
+        <f t="shared" si="19"/>
         <v>0.44086958980801505</v>
       </c>
       <c r="L139">
-        <f>K139/H139</f>
+        <f t="shared" si="20"/>
         <v>1.0396276894333112E-2</v>
       </c>
       <c r="M139" t="s">
@@ -20672,15 +20674,15 @@
       <c r="F140" s="10"/>
       <c r="G140" s="10"/>
       <c r="H140">
-        <f>AVERAGE(C140:F140)</f>
+        <f t="shared" si="21"/>
         <v>54.851871287474033</v>
       </c>
       <c r="K140">
-        <f>_xlfn.STDEV.P(C140:G140)</f>
+        <f t="shared" si="19"/>
         <v>5.2237699148308083</v>
       </c>
       <c r="L140">
-        <f>K140/H140</f>
+        <f t="shared" si="20"/>
         <v>9.5234124054828881E-2</v>
       </c>
       <c r="M140" t="s">
@@ -20712,15 +20714,15 @@
       <c r="F141" s="10"/>
       <c r="G141" s="10"/>
       <c r="H141">
-        <f>AVERAGE(C141:F141)</f>
+        <f t="shared" si="21"/>
         <v>168.32058507783168</v>
       </c>
       <c r="K141">
-        <f>_xlfn.STDEV.P(C141:G141)</f>
+        <f t="shared" si="19"/>
         <v>17.925476681330977</v>
       </c>
       <c r="L141">
-        <f>K141/H141</f>
+        <f t="shared" si="20"/>
         <v>0.10649604546610987</v>
       </c>
       <c r="M141" t="s">
@@ -20752,15 +20754,15 @@
       <c r="F142" s="10"/>
       <c r="G142" s="10"/>
       <c r="H142">
-        <f>AVERAGE(C142:F142)</f>
+        <f t="shared" si="21"/>
         <v>8.3008234039586259</v>
       </c>
       <c r="K142">
-        <f>_xlfn.STDEV.P(C142:G142)</f>
+        <f t="shared" si="19"/>
         <v>3.320320640221361</v>
       </c>
       <c r="L142">
-        <f>K142/H142</f>
+        <f t="shared" si="20"/>
         <v>0.39999894933771446</v>
       </c>
       <c r="M142" t="s">
@@ -20792,15 +20794,15 @@
       <c r="F143" s="10"/>
       <c r="G143" s="10"/>
       <c r="H143">
-        <f>AVERAGE(C143:F143)</f>
+        <f t="shared" si="21"/>
         <v>8.7589714298898276</v>
       </c>
       <c r="K143">
-        <f>_xlfn.STDEV.P(C143:G143)</f>
+        <f t="shared" si="19"/>
         <v>1.8669019599156651</v>
       </c>
       <c r="L143">
-        <f>K143/H143</f>
+        <f t="shared" si="20"/>
         <v>0.21314168848009901</v>
       </c>
       <c r="M143" t="s">
@@ -20832,15 +20834,15 @@
       <c r="F144" s="10"/>
       <c r="G144" s="10"/>
       <c r="H144">
-        <f>AVERAGE(C144:F144)</f>
+        <f t="shared" si="21"/>
         <v>5.7795831952248875</v>
       </c>
       <c r="K144">
-        <f>_xlfn.STDEV.P(C144:G144)</f>
+        <f t="shared" si="19"/>
         <v>1.2673800425040533</v>
       </c>
       <c r="L144">
-        <f>K144/H144</f>
+        <f t="shared" si="20"/>
         <v>0.21928571658094087</v>
       </c>
       <c r="M144" t="s">
@@ -20872,15 +20874,15 @@
       <c r="F145" s="10"/>
       <c r="G145" s="10"/>
       <c r="H145">
-        <f>AVERAGE(C145:F145)</f>
+        <f t="shared" si="21"/>
         <v>6.4601792369234161</v>
       </c>
       <c r="K145">
-        <f>_xlfn.STDEV.P(C145:G145)</f>
+        <f t="shared" si="19"/>
         <v>1.2163083628430251</v>
       </c>
       <c r="L145">
-        <f>K145/H145</f>
+        <f t="shared" si="20"/>
         <v>0.18827780441309824</v>
       </c>
       <c r="M145" t="s">
@@ -20912,15 +20914,15 @@
       <c r="F146" s="10"/>
       <c r="G146" s="10"/>
       <c r="H146">
-        <f>AVERAGE(C146:F146)</f>
+        <f t="shared" si="21"/>
         <v>8.3464931480834377</v>
       </c>
       <c r="K146">
-        <f>_xlfn.STDEV.P(C146:G146)</f>
+        <f t="shared" si="19"/>
         <v>2.9807454298696037</v>
       </c>
       <c r="L146">
-        <f>K146/H146</f>
+        <f t="shared" si="20"/>
         <v>0.35712548695424939</v>
       </c>
       <c r="M146" t="s">
@@ -20952,15 +20954,15 @@
       <c r="F147" s="10"/>
       <c r="G147" s="10"/>
       <c r="H147">
-        <f>AVERAGE(C147:F147)</f>
+        <f t="shared" si="21"/>
         <v>5.6586774852099397</v>
       </c>
       <c r="K147">
-        <f>_xlfn.STDEV.P(C147:G147)</f>
+        <f t="shared" si="19"/>
         <v>2.8391256414819663</v>
       </c>
       <c r="L147">
-        <f>K147/H147</f>
+        <f t="shared" si="20"/>
         <v>0.50172953820085642</v>
       </c>
       <c r="M147" t="s">
@@ -20992,15 +20994,15 @@
       <c r="F148" s="10"/>
       <c r="G148" s="10"/>
       <c r="H148">
-        <f>AVERAGE(C148:F148)</f>
+        <f t="shared" si="21"/>
         <v>6.427442643984854</v>
       </c>
       <c r="K148">
-        <f>_xlfn.STDEV.P(C148:G148)</f>
+        <f t="shared" si="19"/>
         <v>0.75147424950728858</v>
       </c>
       <c r="L148">
-        <f>K148/H148</f>
+        <f t="shared" si="20"/>
         <v>0.11691652358976062</v>
       </c>
       <c r="M148" t="s">
@@ -21032,15 +21034,15 @@
       <c r="F149" s="10"/>
       <c r="G149" s="10"/>
       <c r="H149">
-        <f>AVERAGE(C149:F149)</f>
+        <f t="shared" si="21"/>
         <v>32.746822184306936</v>
       </c>
       <c r="K149">
-        <f>_xlfn.STDEV.P(C149:G149)</f>
+        <f t="shared" si="19"/>
         <v>1.4506638503487761</v>
       </c>
       <c r="L149">
-        <f>K149/H149</f>
+        <f t="shared" si="20"/>
         <v>4.429937788112976E-2</v>
       </c>
       <c r="M149" t="s">
@@ -21072,15 +21074,15 @@
       <c r="F150" s="10"/>
       <c r="G150" s="10"/>
       <c r="H150">
-        <f>AVERAGE(C150:F150)</f>
+        <f t="shared" si="21"/>
         <v>25.349995388837403</v>
       </c>
       <c r="K150">
-        <f>_xlfn.STDEV.P(C150:G150)</f>
+        <f t="shared" si="19"/>
         <v>1.3250079792129639</v>
       </c>
       <c r="L150">
-        <f>K150/H150</f>
+        <f t="shared" si="20"/>
         <v>5.2268568845437222E-2</v>
       </c>
       <c r="M150" t="s">
@@ -21112,15 +21114,15 @@
       <c r="F151" s="10"/>
       <c r="G151" s="10"/>
       <c r="H151">
-        <f>AVERAGE(C151:F151)</f>
+        <f t="shared" si="21"/>
         <v>18.141373789237168</v>
       </c>
       <c r="K151">
-        <f>_xlfn.STDEV.P(C151:G151)</f>
+        <f t="shared" si="19"/>
         <v>1.5049331227111069</v>
       </c>
       <c r="L151">
-        <f>K151/H151</f>
+        <f t="shared" si="20"/>
         <v>8.2955852197034094E-2</v>
       </c>
       <c r="M151" t="s">
@@ -21152,15 +21154,15 @@
       <c r="F152" s="10"/>
       <c r="G152" s="10"/>
       <c r="H152">
-        <f>AVERAGE(C152:F152)</f>
+        <f t="shared" si="21"/>
         <v>23.868746556821634</v>
       </c>
       <c r="K152">
-        <f>_xlfn.STDEV.P(C152:G152)</f>
+        <f t="shared" si="19"/>
         <v>1.8700478579090605</v>
       </c>
       <c r="L152">
-        <f>K152/H152</f>
+        <f t="shared" si="20"/>
         <v>7.8347132869220779E-2</v>
       </c>
       <c r="M152" t="s">
@@ -21192,15 +21194,15 @@
       <c r="F153" s="10"/>
       <c r="G153" s="10"/>
       <c r="H153">
-        <f>AVERAGE(C153:F153)</f>
+        <f t="shared" si="21"/>
         <v>17.3442792621466</v>
       </c>
       <c r="K153">
-        <f>_xlfn.STDEV.P(C153:G153)</f>
+        <f t="shared" si="19"/>
         <v>0.8667499906826277</v>
       </c>
       <c r="L153">
-        <f>K153/H153</f>
+        <f t="shared" si="20"/>
         <v>4.9973249253100135E-2</v>
       </c>
       <c r="M153" t="s">
@@ -21232,15 +21234,15 @@
       <c r="F154" s="10"/>
       <c r="G154" s="10"/>
       <c r="H154">
-        <f>AVERAGE(C154:F154)</f>
+        <f t="shared" si="21"/>
         <v>34.101430245540001</v>
       </c>
       <c r="K154">
-        <f>_xlfn.STDEV.P(C154:G154)</f>
+        <f t="shared" si="19"/>
         <v>2.23404667374612</v>
       </c>
       <c r="L154">
-        <f>K154/H154</f>
+        <f t="shared" si="20"/>
         <v>6.5511817471007761E-2</v>
       </c>
       <c r="M154" t="s">
@@ -21272,15 +21274,15 @@
       <c r="F155" s="10"/>
       <c r="G155" s="10"/>
       <c r="H155">
-        <f>AVERAGE(C155:F155)</f>
+        <f t="shared" si="21"/>
         <v>153.89492753623199</v>
       </c>
       <c r="K155">
-        <f>_xlfn.STDEV.P(C155:G155)</f>
+        <f t="shared" si="19"/>
         <v>15.256341054756252</v>
       </c>
       <c r="L155">
-        <f>K155/H155</f>
+        <f t="shared" si="20"/>
         <v>9.9134788254566744E-2</v>
       </c>
       <c r="M155" t="s">
@@ -21312,15 +21314,15 @@
       <c r="F156" s="10"/>
       <c r="G156" s="10"/>
       <c r="H156">
-        <f>AVERAGE(C156:F156)</f>
+        <f t="shared" si="21"/>
         <v>9.7692930953545591</v>
       </c>
       <c r="K156">
-        <f>_xlfn.STDEV.P(C156:G156)</f>
+        <f t="shared" si="19"/>
         <v>2.9962163590068829</v>
       </c>
       <c r="L156">
-        <f>K156/H156</f>
+        <f t="shared" si="20"/>
         <v>0.30669735565940048</v>
       </c>
       <c r="M156" t="s">
@@ -21352,15 +21354,15 @@
       <c r="F157" s="10"/>
       <c r="G157" s="10"/>
       <c r="H157">
-        <f>AVERAGE(C157:F157)</f>
+        <f t="shared" si="21"/>
         <v>18.554495759732532</v>
       </c>
       <c r="K157">
-        <f>_xlfn.STDEV.P(C157:G157)</f>
+        <f t="shared" si="19"/>
         <v>0.51505109057371057</v>
       </c>
       <c r="L157">
-        <f>K157/H157</f>
+        <f t="shared" si="20"/>
         <v>2.7758829840662573E-2</v>
       </c>
       <c r="M157" t="s">
@@ -21392,15 +21394,15 @@
       <c r="F158" s="10"/>
       <c r="G158" s="10"/>
       <c r="H158">
-        <f>AVERAGE(C158:F158)</f>
+        <f t="shared" si="21"/>
         <v>8.8012579216006781</v>
       </c>
       <c r="K158">
-        <f>_xlfn.STDEV.P(C158:G158)</f>
+        <f t="shared" si="19"/>
         <v>2.1727382152639021</v>
       </c>
       <c r="L158">
-        <f>K158/H158</f>
+        <f t="shared" si="20"/>
         <v>0.24686678138717105</v>
       </c>
       <c r="M158" t="s">
@@ -21432,15 +21434,15 @@
       <c r="F159" s="10"/>
       <c r="G159" s="10"/>
       <c r="H159">
-        <f>AVERAGE(C159:F159)</f>
+        <f t="shared" si="21"/>
         <v>30.886721076742834</v>
       </c>
       <c r="K159">
-        <f>_xlfn.STDEV.P(C159:G159)</f>
+        <f t="shared" si="19"/>
         <v>1.9061097922690926</v>
       </c>
       <c r="L159">
-        <f>K159/H159</f>
+        <f t="shared" si="20"/>
         <v>6.1712921469814427E-2</v>
       </c>
       <c r="M159" t="s">
@@ -21472,15 +21474,15 @@
       <c r="F160" s="10"/>
       <c r="G160" s="10"/>
       <c r="H160">
-        <f>AVERAGE(C160:F160)</f>
+        <f t="shared" si="21"/>
         <v>11.867361121928283</v>
       </c>
       <c r="K160">
-        <f>_xlfn.STDEV.P(C160:G160)</f>
+        <f t="shared" si="19"/>
         <v>1.9413417484395468</v>
       </c>
       <c r="L160">
-        <f>K160/H160</f>
+        <f t="shared" si="20"/>
         <v>0.16358664141873736</v>
       </c>
       <c r="M160" t="s">
@@ -21512,15 +21514,15 @@
       <c r="F161" s="10"/>
       <c r="G161" s="10"/>
       <c r="H161">
-        <f>AVERAGE(C161:F161)</f>
+        <f t="shared" si="21"/>
         <v>35.678729882178132</v>
       </c>
       <c r="K161">
-        <f>_xlfn.STDEV.P(C161:G161)</f>
+        <f t="shared" si="19"/>
         <v>3.5401825704095962</v>
       </c>
       <c r="L161">
-        <f>K161/H161</f>
+        <f t="shared" si="20"/>
         <v>9.9223895640353249E-2</v>
       </c>
       <c r="M161" t="s">
@@ -21552,15 +21554,15 @@
       <c r="F162" s="10"/>
       <c r="G162" s="10"/>
       <c r="H162">
-        <f>AVERAGE(C162:F162)</f>
+        <f t="shared" si="21"/>
         <v>17.525054268894568</v>
       </c>
       <c r="K162">
-        <f>_xlfn.STDEV.P(C162:G162)</f>
+        <f t="shared" ref="K162:K179" si="22">_xlfn.STDEV.P(C162:G162)</f>
         <v>1.3467453001412995</v>
       </c>
       <c r="L162">
-        <f>K162/H162</f>
+        <f t="shared" ref="L162:L193" si="23">K162/H162</f>
         <v>7.6846854764475919E-2</v>
       </c>
       <c r="M162" t="s">
@@ -21592,15 +21594,15 @@
       <c r="F163" s="10"/>
       <c r="G163" s="10"/>
       <c r="H163">
-        <f>AVERAGE(C163:F163)</f>
+        <f t="shared" si="21"/>
         <v>17.354002372198934</v>
       </c>
       <c r="K163">
-        <f>_xlfn.STDEV.P(C163:G163)</f>
+        <f t="shared" si="22"/>
         <v>0.75896121002842498</v>
       </c>
       <c r="L163">
-        <f>K163/H163</f>
+        <f t="shared" si="23"/>
         <v>4.3734073198254189E-2</v>
       </c>
       <c r="M163" t="s">
@@ -21632,15 +21634,15 @@
       <c r="F164" s="10"/>
       <c r="G164" s="10"/>
       <c r="H164">
-        <f>AVERAGE(C164:F164)</f>
+        <f t="shared" si="21"/>
         <v>22.768179465059635</v>
       </c>
       <c r="K164">
-        <f>_xlfn.STDEV.P(C164:G164)</f>
+        <f t="shared" si="22"/>
         <v>7.4605573725537652E-2</v>
       </c>
       <c r="L164">
-        <f>K164/H164</f>
+        <f t="shared" si="23"/>
         <v>3.2767474378014457E-3</v>
       </c>
       <c r="M164" t="s">
@@ -21672,15 +21674,15 @@
       <c r="F165" s="10"/>
       <c r="G165" s="10"/>
       <c r="H165">
-        <f>AVERAGE(C165:F165)</f>
+        <f t="shared" si="21"/>
         <v>19.218269064439934</v>
       </c>
       <c r="K165">
-        <f>_xlfn.STDEV.P(C165:G165)</f>
+        <f t="shared" si="22"/>
         <v>1.347754250918602</v>
       </c>
       <c r="L165">
-        <f>K165/H165</f>
+        <f t="shared" si="23"/>
         <v>7.0128805377815587E-2</v>
       </c>
       <c r="M165" t="s">
@@ -21712,15 +21714,15 @@
       <c r="F166" s="10"/>
       <c r="G166" s="10"/>
       <c r="H166">
-        <f>AVERAGE(C166:F166)</f>
+        <f t="shared" si="21"/>
         <v>158.133544043581</v>
       </c>
       <c r="K166">
-        <f>_xlfn.STDEV.P(C166:G166)</f>
+        <f t="shared" si="22"/>
         <v>15.670235879747452</v>
       </c>
       <c r="L166">
-        <f>K166/H166</f>
+        <f t="shared" si="23"/>
         <v>9.9094951514074672E-2</v>
       </c>
       <c r="M166" t="s">
@@ -21752,15 +21754,15 @@
       <c r="F167" s="10"/>
       <c r="G167" s="10"/>
       <c r="H167">
-        <f>AVERAGE(C167:F167)</f>
+        <f t="shared" si="21"/>
         <v>14.835455810456834</v>
       </c>
       <c r="K167">
-        <f>_xlfn.STDEV.P(C167:G167)</f>
+        <f t="shared" si="22"/>
         <v>0.31744674737713491</v>
       </c>
       <c r="L167">
-        <f>K167/H167</f>
+        <f t="shared" si="23"/>
         <v>2.1397842535676E-2</v>
       </c>
       <c r="M167" t="s">
@@ -21792,15 +21794,15 @@
       <c r="F168" s="10"/>
       <c r="G168" s="10"/>
       <c r="H168">
-        <f>AVERAGE(C168:F168)</f>
+        <f t="shared" si="21"/>
         <v>164.81010381334167</v>
       </c>
       <c r="K168">
-        <f>_xlfn.STDEV.P(C168:G168)</f>
+        <f t="shared" si="22"/>
         <v>6.8706934839678295</v>
       </c>
       <c r="L168">
-        <f>K168/H168</f>
+        <f t="shared" si="23"/>
         <v>4.1688545331840479E-2</v>
       </c>
       <c r="M168" t="s">
@@ -21832,15 +21834,15 @@
       <c r="F169" s="10"/>
       <c r="G169" s="10"/>
       <c r="H169">
-        <f>AVERAGE(C169:F169)</f>
+        <f t="shared" si="21"/>
         <v>21.074682354896229</v>
       </c>
       <c r="K169">
-        <f>_xlfn.STDEV.P(C169:G169)</f>
+        <f t="shared" si="22"/>
         <v>1.2487606314942454</v>
       </c>
       <c r="L169">
-        <f>K169/H169</f>
+        <f t="shared" si="23"/>
         <v>5.9254066584027251E-2</v>
       </c>
       <c r="M169" t="s">
@@ -21872,15 +21874,15 @@
       <c r="F170" s="10"/>
       <c r="G170" s="10"/>
       <c r="H170">
-        <f>AVERAGE(C170:F170)</f>
+        <f t="shared" ref="H170:H179" si="24">AVERAGE(C170:F170)</f>
         <v>152.27187332259834</v>
       </c>
       <c r="K170">
-        <f>_xlfn.STDEV.P(C170:G170)</f>
+        <f t="shared" si="22"/>
         <v>18.231268370011271</v>
       </c>
       <c r="L170">
-        <f>K170/H170</f>
+        <f t="shared" si="23"/>
         <v>0.11972840401974361</v>
       </c>
       <c r="M170" t="s">
@@ -21912,15 +21914,15 @@
       <c r="F171" s="10"/>
       <c r="G171" s="10"/>
       <c r="H171">
-        <f>AVERAGE(C171:F171)</f>
+        <f t="shared" si="24"/>
         <v>31.565529677918803</v>
       </c>
       <c r="K171">
-        <f>_xlfn.STDEV.P(C171:G171)</f>
+        <f t="shared" si="22"/>
         <v>1.2578853019832938</v>
       </c>
       <c r="L171">
-        <f>K171/H171</f>
+        <f t="shared" si="23"/>
         <v>3.9849966555867075E-2</v>
       </c>
       <c r="M171" t="s">
@@ -21952,15 +21954,15 @@
       <c r="F172" s="10"/>
       <c r="G172" s="10"/>
       <c r="H172">
-        <f>AVERAGE(C172:F172)</f>
+        <f t="shared" si="24"/>
         <v>14.732158495904132</v>
       </c>
       <c r="K172">
-        <f>_xlfn.STDEV.P(C172:G172)</f>
+        <f t="shared" si="22"/>
         <v>1.3514886554144694</v>
       </c>
       <c r="L172">
-        <f>K172/H172</f>
+        <f t="shared" si="23"/>
         <v>9.1737314378623702E-2</v>
       </c>
       <c r="M172" t="s">
@@ -21992,15 +21994,15 @@
       <c r="F173" s="10"/>
       <c r="G173" s="10"/>
       <c r="H173">
-        <f>AVERAGE(C173:F173)</f>
+        <f t="shared" si="24"/>
         <v>26.166945453428436</v>
       </c>
       <c r="K173">
-        <f>_xlfn.STDEV.P(C173:G173)</f>
+        <f t="shared" si="22"/>
         <v>3.4618057796778205</v>
       </c>
       <c r="L173">
-        <f>K173/H173</f>
+        <f t="shared" si="23"/>
         <v>0.13229690052433113</v>
       </c>
       <c r="M173" t="s">
@@ -22032,15 +22034,15 @@
       <c r="F174" s="10"/>
       <c r="G174" s="10"/>
       <c r="H174">
-        <f>AVERAGE(C174:F174)</f>
+        <f t="shared" si="24"/>
         <v>16.652406594370564</v>
       </c>
       <c r="K174">
-        <f>_xlfn.STDEV.P(C174:G174)</f>
+        <f t="shared" si="22"/>
         <v>0.94854149746010141</v>
       </c>
       <c r="L174">
-        <f>K174/H174</f>
+        <f t="shared" si="23"/>
         <v>5.696122611975863E-2</v>
       </c>
       <c r="M174" t="s">
@@ -22072,15 +22074,15 @@
       <c r="F175" s="10"/>
       <c r="G175" s="10"/>
       <c r="H175">
-        <f>AVERAGE(C175:F175)</f>
+        <f t="shared" si="24"/>
         <v>46.109290348969466</v>
       </c>
       <c r="K175">
-        <f>_xlfn.STDEV.P(C175:G175)</f>
+        <f t="shared" si="22"/>
         <v>2.1850415759889743</v>
       </c>
       <c r="L175">
-        <f>K175/H175</f>
+        <f t="shared" si="23"/>
         <v>4.7388315010964153E-2</v>
       </c>
       <c r="M175" t="s">
@@ -22112,15 +22114,15 @@
       <c r="F176" s="10"/>
       <c r="G176" s="10"/>
       <c r="H176">
-        <f>AVERAGE(C176:F176)</f>
+        <f t="shared" si="24"/>
         <v>26.184307699953802</v>
       </c>
       <c r="K176">
-        <f>_xlfn.STDEV.P(C176:G176)</f>
+        <f t="shared" si="22"/>
         <v>1.4132479812142704</v>
       </c>
       <c r="L176">
-        <f>K176/H176</f>
+        <f t="shared" si="23"/>
         <v>5.397308943236883E-2</v>
       </c>
       <c r="M176" t="s">
@@ -22152,15 +22154,15 @@
       <c r="F177" s="10"/>
       <c r="G177" s="10"/>
       <c r="H177">
-        <f>AVERAGE(C177:F177)</f>
+        <f t="shared" si="24"/>
         <v>19.470232726221166</v>
       </c>
       <c r="K177">
-        <f>_xlfn.STDEV.P(C177:G177)</f>
+        <f t="shared" si="22"/>
         <v>0.49192270061862337</v>
       </c>
       <c r="L177">
-        <f>K177/H177</f>
+        <f t="shared" si="23"/>
         <v>2.526537343111137E-2</v>
       </c>
       <c r="M177" t="s">
@@ -22192,15 +22194,15 @@
       <c r="F178" s="10"/>
       <c r="G178" s="10"/>
       <c r="H178">
-        <f>AVERAGE(C178:F178)</f>
+        <f t="shared" si="24"/>
         <v>18.636131114644069</v>
       </c>
       <c r="K178">
-        <f>_xlfn.STDEV.P(C178:G178)</f>
+        <f t="shared" si="22"/>
         <v>1.1810257108490159</v>
       </c>
       <c r="L178">
-        <f>K178/H178</f>
+        <f t="shared" si="23"/>
         <v>6.3372902003301465E-2</v>
       </c>
       <c r="M178" t="s">
@@ -22232,15 +22234,15 @@
       <c r="F179" s="10"/>
       <c r="G179" s="10"/>
       <c r="H179">
-        <f>AVERAGE(C179:F179)</f>
+        <f t="shared" si="24"/>
         <v>20.534437657695936</v>
       </c>
       <c r="K179">
-        <f>_xlfn.STDEV.P(C179:G179)</f>
+        <f t="shared" si="22"/>
         <v>0.34181402720053022</v>
       </c>
       <c r="L179">
-        <f>K179/H179</f>
+        <f t="shared" si="23"/>
         <v>1.6645891789124526E-2</v>
       </c>
       <c r="M179" t="s">
@@ -22283,11 +22285,11 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>